<commit_message>
working example for pressure
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett Rhyne\Documents\SWWA_Connectivity\Analysis\SWWA_Pressure-main\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raphael/Documents/GitHub/SWWA_Pressure/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FDC70AE-D8C8-4F84-AC73-B3ED7F613033}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3467A6F7-8562-8C42-A030-31F49A28A37B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28935" yWindow="1080" windowWidth="24360" windowHeight="11025" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tracks" sheetId="1" r:id="rId1"/>
@@ -208,9 +208,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yy"/>
-  </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -726,7 +723,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -735,8 +732,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -791,6 +787,42 @@
   </cellStyles>
   <dxfs count="17">
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -815,42 +847,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -925,20 +921,20 @@
     <tableColumn id="51" xr3:uid="{AD7A8CAB-A777-7C4D-A6A2-601A4074FBB2}" name="prob_map_thr"/>
     <tableColumn id="42" xr3:uid="{BF18370D-EF9D-424D-B4AE-3A176A692D5A}" name="shift_k" dataDxfId="14"/>
     <tableColumn id="11" xr3:uid="{85327B51-BF51-A643-9746-0720CC021C70}" name="kernel_adjust"/>
-    <tableColumn id="9" xr3:uid="{0D248294-1CA3-E44D-A900-569DE950BA49}" name="calib_lon" dataDxfId="1"/>
-    <tableColumn id="10" xr3:uid="{50C46AB1-CB9A-B84C-B41F-D6DF90BD8412}" name="calib_lat" dataDxfId="0"/>
-    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="13"/>
-    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="12"/>
-    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="11"/>
-    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="10"/>
-    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="9"/>
-    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="3"/>
-    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{0D248294-1CA3-E44D-A900-569DE950BA49}" name="calib_lon" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{50C46AB1-CB9A-B84C-B41F-D6DF90BD8412}" name="calib_lat" dataDxfId="12"/>
+    <tableColumn id="19" xr3:uid="{F555DC9A-9393-234D-92AB-138553DAA03D}" name="calib_1_start" dataDxfId="11"/>
+    <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="10"/>
+    <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="9"/>
+    <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="8"/>
+    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="7"/>
+    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="1"/>
+    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name"/>
     <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name"/>
     <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass"/>
@@ -1248,26 +1244,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="10.6640625" customWidth="1"/>
     <col min="5" max="5" width="13.1640625" customWidth="1"/>
     <col min="6" max="6" width="14.1640625" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" customWidth="1"/>
-    <col min="8" max="8" width="16.4140625" customWidth="1"/>
-    <col min="9" max="9" width="19.9140625" customWidth="1"/>
-    <col min="10" max="10" width="19.75" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
     <col min="11" max="11" width="16.1640625" customWidth="1"/>
-    <col min="12" max="12" width="15.9140625" customWidth="1"/>
+    <col min="12" max="12" width="15.83203125" customWidth="1"/>
     <col min="13" max="13" width="21.33203125" customWidth="1"/>
-    <col min="14" max="14" width="18.75" customWidth="1"/>
+    <col min="14" max="14" width="18.6640625" customWidth="1"/>
     <col min="15" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="15.1640625" style="9" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" style="9" customWidth="1"/>
+    <col min="17" max="17" width="15.1640625" style="8" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" style="8" customWidth="1"/>
     <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="15.1640625" customWidth="1"/>
@@ -1286,7 +1282,7 @@
     <col min="50" max="50" width="15.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -1335,10 +1331,10 @@
       <c r="P1" t="s">
         <v>31</v>
       </c>
-      <c r="Q1" s="9" t="s">
+      <c r="Q1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="9" t="s">
+      <c r="R1" s="8" t="s">
         <v>7</v>
       </c>
       <c r="S1" t="s">
@@ -1393,7 +1389,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -1404,7 +1400,7 @@
         <v>43222</v>
       </c>
       <c r="D2" s="3">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>50</v>
@@ -1439,10 +1435,10 @@
       <c r="P2">
         <v>1.4</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="Q2" s="8">
         <v>17.05</v>
       </c>
-      <c r="R2" s="9">
+      <c r="R2" s="8">
         <v>48.9</v>
       </c>
       <c r="S2" s="1">
@@ -1478,17 +1474,19 @@
       </c>
       <c r="AI2" s="2"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="7">
         <v>44362</v>
       </c>
-      <c r="C3" s="8">
+      <c r="C3" s="7">
         <v>44702</v>
       </c>
-      <c r="D3" s="6"/>
+      <c r="D3" s="3">
+        <v>0</v>
+      </c>
       <c r="E3" s="5">
         <v>45</v>
       </c>
@@ -1514,31 +1512,47 @@
         <v>1</v>
       </c>
       <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="9">
+      <c r="N3">
+        <v>0.9</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>1.4</v>
+      </c>
+      <c r="Q3" s="8">
         <v>-80.447980000000001</v>
       </c>
-      <c r="R3" s="10">
+      <c r="R3" s="9">
         <v>32.768059999999998</v>
       </c>
-      <c r="S3" s="7">
+      <c r="S3" s="6">
         <v>44363</v>
       </c>
-      <c r="T3" s="7">
+      <c r="T3" s="6">
         <v>44418</v>
       </c>
-      <c r="U3" s="7"/>
-      <c r="V3" s="7"/>
-      <c r="W3" s="7"/>
-      <c r="X3" s="7"/>
-      <c r="Y3" s="6"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="6"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="6"/>
-      <c r="AD3" s="7"/>
+      <c r="U3" s="6"/>
+      <c r="V3" s="6"/>
+      <c r="W3" s="6"/>
+      <c r="X3" s="6"/>
+      <c r="Y3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z3" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA3" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB3" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC3" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD3" s="6"/>
       <c r="AE3" s="5" t="s">
         <v>55</v>
       </c>
@@ -1549,17 +1563,19 @@
       <c r="AH3" s="5"/>
       <c r="AI3" s="5"/>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B4" s="8">
+      <c r="B4" s="7">
         <v>44362</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="7">
         <v>44671</v>
       </c>
-      <c r="D4" s="6"/>
+      <c r="D4" s="3">
+        <v>0</v>
+      </c>
       <c r="E4" s="5">
         <v>45</v>
       </c>
@@ -1585,31 +1601,47 @@
         <v>1</v>
       </c>
       <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="10">
+      <c r="N4">
+        <v>0.9</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>1.4</v>
+      </c>
+      <c r="Q4" s="9">
         <v>-80.354759999999999</v>
       </c>
-      <c r="R4" s="9">
+      <c r="R4" s="8">
         <v>33.219625999999998</v>
       </c>
-      <c r="S4" s="7">
+      <c r="S4" s="6">
         <v>44363</v>
       </c>
-      <c r="T4" s="7">
+      <c r="T4" s="6">
         <v>44418</v>
       </c>
-      <c r="U4" s="7"/>
-      <c r="V4" s="7"/>
-      <c r="W4" s="7"/>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="6"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="6"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="6"/>
-      <c r="AD4" s="7"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA4" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB4" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC4" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD4" s="6"/>
       <c r="AE4" s="5" t="s">
         <v>55</v>
       </c>
@@ -1620,17 +1652,19 @@
       <c r="AH4" s="5"/>
       <c r="AI4" s="5"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B5" s="8">
+      <c r="B5" s="7">
         <v>44362</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="7">
         <v>44721</v>
       </c>
-      <c r="D5" s="6"/>
+      <c r="D5" s="3">
+        <v>0</v>
+      </c>
       <c r="E5" s="5">
         <v>45</v>
       </c>
@@ -1656,31 +1690,47 @@
         <v>1</v>
       </c>
       <c r="M5" s="5"/>
-      <c r="N5" s="5"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="5"/>
-      <c r="Q5" s="11">
+      <c r="N5">
+        <v>0.9</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>1.4</v>
+      </c>
+      <c r="Q5" s="10">
         <v>-84.179299999999998</v>
       </c>
-      <c r="R5" s="11">
+      <c r="R5" s="10">
         <v>35.285809999999998</v>
       </c>
-      <c r="S5" s="7">
+      <c r="S5" s="6">
         <v>44363</v>
       </c>
-      <c r="T5" s="7">
+      <c r="T5" s="6">
         <v>44418</v>
       </c>
-      <c r="U5" s="7"/>
-      <c r="V5" s="7"/>
-      <c r="W5" s="7"/>
-      <c r="X5" s="7"/>
-      <c r="Y5" s="6"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="6"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="6"/>
-      <c r="AD5" s="7"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC5" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD5" s="6"/>
       <c r="AE5" s="5" t="s">
         <v>55</v>
       </c>
@@ -1691,17 +1741,19 @@
       <c r="AH5" s="5"/>
       <c r="AI5" s="5"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="8">
+      <c r="B6" s="7">
         <v>44362</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="7">
         <v>44697</v>
       </c>
-      <c r="D6" s="6"/>
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
       <c r="E6" s="5">
         <v>45</v>
       </c>
@@ -1727,31 +1779,47 @@
         <v>1</v>
       </c>
       <c r="M6" s="5"/>
-      <c r="N6" s="5"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="5"/>
-      <c r="Q6" s="11">
+      <c r="N6">
+        <v>0.9</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>1.4</v>
+      </c>
+      <c r="Q6" s="10">
         <v>-84.049199999999999</v>
       </c>
-      <c r="R6" s="11">
+      <c r="R6" s="10">
         <v>35.439259999999997</v>
       </c>
-      <c r="S6" s="7">
+      <c r="S6" s="6">
         <v>44363</v>
       </c>
-      <c r="T6" s="7">
+      <c r="T6" s="6">
         <v>44418</v>
       </c>
-      <c r="U6" s="7"/>
-      <c r="V6" s="7"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="7"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="6"/>
-      <c r="AD6" s="7"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA6" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB6" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC6" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD6" s="6"/>
       <c r="AE6" s="5" t="s">
         <v>55</v>
       </c>
@@ -1762,17 +1830,19 @@
       <c r="AH6" s="5"/>
       <c r="AI6" s="5"/>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="B7" s="8">
+      <c r="B7" s="7">
         <v>44362</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="7">
         <v>44716</v>
       </c>
-      <c r="D7" s="6"/>
+      <c r="D7" s="3">
+        <v>0</v>
+      </c>
       <c r="E7" s="5">
         <v>45</v>
       </c>
@@ -1798,31 +1868,47 @@
         <v>1</v>
       </c>
       <c r="M7" s="5"/>
-      <c r="N7" s="5"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="5"/>
-      <c r="Q7" s="11">
+      <c r="N7">
+        <v>0.9</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>1.4</v>
+      </c>
+      <c r="Q7" s="10">
         <v>-84.049199999999999</v>
       </c>
-      <c r="R7" s="11">
+      <c r="R7" s="10">
         <v>35.439259999999997</v>
       </c>
-      <c r="S7" s="7">
+      <c r="S7" s="6">
         <v>44363</v>
       </c>
-      <c r="T7" s="7">
+      <c r="T7" s="6">
         <v>44418</v>
       </c>
-      <c r="U7" s="7"/>
-      <c r="V7" s="7"/>
-      <c r="W7" s="7"/>
-      <c r="X7" s="7"/>
-      <c r="Y7" s="6"/>
-      <c r="Z7" s="6"/>
-      <c r="AA7" s="6"/>
-      <c r="AB7" s="6"/>
-      <c r="AC7" s="6"/>
-      <c r="AD7" s="7"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA7" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB7" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC7" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD7" s="6"/>
       <c r="AE7" s="5" t="s">
         <v>55</v>
       </c>
@@ -1833,17 +1919,19 @@
       <c r="AH7" s="5"/>
       <c r="AI7" s="5"/>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="8">
+      <c r="B8" s="7">
         <v>44362</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="7">
         <v>44724</v>
       </c>
-      <c r="D8" s="6"/>
+      <c r="D8" s="3">
+        <v>0</v>
+      </c>
       <c r="E8" s="5">
         <v>45</v>
       </c>
@@ -1869,31 +1957,47 @@
         <v>1</v>
       </c>
       <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
-      <c r="O8" s="6"/>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="9">
+      <c r="N8">
+        <v>0.9</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>1.4</v>
+      </c>
+      <c r="Q8" s="8">
         <v>-82.48312</v>
       </c>
-      <c r="R8" s="9">
+      <c r="R8" s="8">
         <v>37.218330000000002</v>
       </c>
-      <c r="S8" s="7">
+      <c r="S8" s="6">
         <v>44363</v>
       </c>
-      <c r="T8" s="7">
+      <c r="T8" s="6">
         <v>44418</v>
       </c>
-      <c r="U8" s="7"/>
-      <c r="V8" s="7"/>
-      <c r="W8" s="7"/>
-      <c r="X8" s="7"/>
-      <c r="Y8" s="6"/>
-      <c r="Z8" s="6"/>
-      <c r="AA8" s="6"/>
-      <c r="AB8" s="6"/>
-      <c r="AC8" s="6"/>
-      <c r="AD8" s="7"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA8" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB8" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC8" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD8" s="6"/>
       <c r="AE8" s="5" t="s">
         <v>55</v>
       </c>
@@ -1904,17 +2008,19 @@
       <c r="AH8" s="5"/>
       <c r="AI8" s="5"/>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="7">
         <v>44362</v>
       </c>
-      <c r="C9" s="8">
+      <c r="C9" s="7">
         <v>44684</v>
       </c>
-      <c r="D9" s="6"/>
+      <c r="D9" s="3">
+        <v>0</v>
+      </c>
       <c r="E9" s="5">
         <v>45</v>
       </c>
@@ -1940,31 +2046,47 @@
         <v>1</v>
       </c>
       <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="6"/>
-      <c r="P9" s="5"/>
-      <c r="Q9" s="9">
+      <c r="N9">
+        <v>0.9</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>1.4</v>
+      </c>
+      <c r="Q9" s="8">
         <v>-91.196119999999993</v>
       </c>
-      <c r="R9" s="9">
+      <c r="R9" s="8">
         <v>36.663780000000003</v>
       </c>
-      <c r="S9" s="7">
+      <c r="S9" s="6">
         <v>44363</v>
       </c>
-      <c r="T9" s="7">
+      <c r="T9" s="6">
         <v>44418</v>
       </c>
-      <c r="U9" s="7"/>
-      <c r="V9" s="7"/>
-      <c r="W9" s="7"/>
-      <c r="X9" s="7"/>
-      <c r="Y9" s="6"/>
-      <c r="Z9" s="6"/>
-      <c r="AA9" s="6"/>
-      <c r="AB9" s="6"/>
-      <c r="AC9" s="6"/>
-      <c r="AD9" s="7"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA9" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB9" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC9" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD9" s="6"/>
       <c r="AE9" s="5" t="s">
         <v>55</v>
       </c>
@@ -1975,17 +2097,19 @@
       <c r="AH9" s="5"/>
       <c r="AI9" s="5"/>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B10" s="8">
+      <c r="B10" s="7">
         <v>44362</v>
       </c>
-      <c r="C10" s="8">
+      <c r="C10" s="7">
         <v>44724</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="3">
+        <v>0</v>
+      </c>
       <c r="E10" s="5">
         <v>45</v>
       </c>
@@ -2011,31 +2135,47 @@
         <v>1</v>
       </c>
       <c r="M10" s="5"/>
-      <c r="N10" s="5"/>
-      <c r="O10" s="6"/>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="9">
+      <c r="N10">
+        <v>0.9</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>1.4</v>
+      </c>
+      <c r="Q10" s="8">
         <v>-82.479211000000006</v>
       </c>
-      <c r="R10" s="9">
+      <c r="R10" s="8">
         <v>37.215834999999998</v>
       </c>
-      <c r="S10" s="7">
+      <c r="S10" s="6">
         <v>44363</v>
       </c>
-      <c r="T10" s="7">
+      <c r="T10" s="6">
         <v>44418</v>
       </c>
-      <c r="U10" s="7"/>
-      <c r="V10" s="7"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="7"/>
-      <c r="Y10" s="6"/>
-      <c r="Z10" s="6"/>
-      <c r="AA10" s="6"/>
-      <c r="AB10" s="6"/>
-      <c r="AC10" s="6"/>
-      <c r="AD10" s="7"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC10" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD10" s="6"/>
       <c r="AE10" s="5" t="s">
         <v>55</v>
       </c>
@@ -2046,17 +2186,19 @@
       <c r="AH10" s="5"/>
       <c r="AI10" s="5"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="7">
         <v>44362</v>
       </c>
-      <c r="C11" s="8">
+      <c r="C11" s="7">
         <v>44684</v>
       </c>
-      <c r="D11" s="6"/>
+      <c r="D11" s="3">
+        <v>0</v>
+      </c>
       <c r="E11" s="5">
         <v>45</v>
       </c>
@@ -2082,31 +2224,47 @@
         <v>1</v>
       </c>
       <c r="M11" s="5"/>
-      <c r="N11" s="5"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="9">
+      <c r="N11">
+        <v>0.9</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>1.4</v>
+      </c>
+      <c r="Q11" s="8">
         <v>-91.197329999999994</v>
       </c>
-      <c r="R11" s="9">
+      <c r="R11" s="8">
         <v>36.650010000000002</v>
       </c>
-      <c r="S11" s="7">
+      <c r="S11" s="6">
         <v>44363</v>
       </c>
-      <c r="T11" s="7">
+      <c r="T11" s="6">
         <v>44418</v>
       </c>
-      <c r="U11" s="7"/>
-      <c r="V11" s="7"/>
-      <c r="W11" s="7"/>
-      <c r="X11" s="7"/>
-      <c r="Y11" s="6"/>
-      <c r="Z11" s="6"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="6"/>
-      <c r="AC11" s="6"/>
-      <c r="AD11" s="7"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD11" s="6"/>
       <c r="AE11" s="5" t="s">
         <v>55</v>
       </c>
@@ -2117,17 +2275,19 @@
       <c r="AH11" s="5"/>
       <c r="AI11" s="5"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="7">
         <v>44362</v>
       </c>
-      <c r="C12" s="8">
+      <c r="C12" s="7">
         <v>44685</v>
       </c>
-      <c r="D12" s="6"/>
+      <c r="D12" s="3">
+        <v>0</v>
+      </c>
       <c r="E12" s="5">
         <v>45</v>
       </c>
@@ -2153,31 +2313,47 @@
         <v>1</v>
       </c>
       <c r="M12" s="5"/>
-      <c r="N12" s="5"/>
-      <c r="O12" s="6"/>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="9">
+      <c r="N12">
+        <v>0.9</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>1.4</v>
+      </c>
+      <c r="Q12" s="8">
         <v>-91.214569999999995</v>
       </c>
-      <c r="R12" s="9">
+      <c r="R12" s="8">
         <v>36.732098999999998</v>
       </c>
-      <c r="S12" s="7">
+      <c r="S12" s="6">
         <v>44363</v>
       </c>
-      <c r="T12" s="7">
+      <c r="T12" s="6">
         <v>44418</v>
       </c>
-      <c r="U12" s="7"/>
-      <c r="V12" s="7"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="7"/>
-      <c r="Y12" s="6"/>
-      <c r="Z12" s="6"/>
-      <c r="AA12" s="6"/>
-      <c r="AB12" s="6"/>
-      <c r="AC12" s="6"/>
-      <c r="AD12" s="7"/>
+      <c r="U12" s="6"/>
+      <c r="V12" s="6"/>
+      <c r="W12" s="6"/>
+      <c r="X12" s="6"/>
+      <c r="Y12" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD12" s="6"/>
       <c r="AE12" s="5" t="s">
         <v>55</v>
       </c>
@@ -2188,17 +2364,19 @@
       <c r="AH12" s="5"/>
       <c r="AI12" s="5"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B13" s="8">
+      <c r="B13" s="7">
         <v>44362</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="7">
         <v>44726</v>
       </c>
-      <c r="D13" s="6"/>
+      <c r="D13" s="3">
+        <v>0</v>
+      </c>
       <c r="E13" s="5">
         <v>45</v>
       </c>
@@ -2224,31 +2402,47 @@
         <v>1</v>
       </c>
       <c r="M13" s="5"/>
-      <c r="N13" s="5"/>
-      <c r="O13" s="6"/>
-      <c r="P13" s="5"/>
-      <c r="Q13" s="9">
+      <c r="N13">
+        <v>0.9</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+      <c r="P13">
+        <v>1.4</v>
+      </c>
+      <c r="Q13" s="8">
         <v>-82.301767999999996</v>
       </c>
-      <c r="R13" s="9">
+      <c r="R13" s="8">
         <v>37.294294999999998</v>
       </c>
-      <c r="S13" s="7">
+      <c r="S13" s="6">
         <v>44378</v>
       </c>
-      <c r="T13" s="7">
+      <c r="T13" s="6">
         <v>44418</v>
       </c>
-      <c r="U13" s="7"/>
-      <c r="V13" s="7"/>
-      <c r="W13" s="7"/>
-      <c r="X13" s="7"/>
-      <c r="Y13" s="6"/>
-      <c r="Z13" s="6"/>
-      <c r="AA13" s="6"/>
-      <c r="AB13" s="6"/>
-      <c r="AC13" s="6"/>
-      <c r="AD13" s="7"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6"/>
+      <c r="W13" s="6"/>
+      <c r="X13" s="6"/>
+      <c r="Y13" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC13" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD13" s="6"/>
       <c r="AE13" s="5" t="s">
         <v>55</v>
       </c>
@@ -2259,17 +2453,19 @@
       <c r="AH13" s="5"/>
       <c r="AI13" s="5"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="7">
         <v>44362</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <v>44722</v>
       </c>
-      <c r="D14" s="6"/>
+      <c r="D14" s="3">
+        <v>0</v>
+      </c>
       <c r="E14" s="5">
         <v>45</v>
       </c>
@@ -2295,31 +2491,47 @@
         <v>1</v>
       </c>
       <c r="M14" s="5"/>
-      <c r="N14" s="5"/>
-      <c r="O14" s="6"/>
-      <c r="P14" s="5"/>
-      <c r="Q14" s="9">
+      <c r="N14">
+        <v>0.9</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>1.4</v>
+      </c>
+      <c r="Q14" s="8">
         <v>-82.304972000000006</v>
       </c>
-      <c r="R14" s="9">
+      <c r="R14" s="8">
         <v>37.286811999999998</v>
       </c>
-      <c r="S14" s="7">
+      <c r="S14" s="6">
         <v>44378</v>
       </c>
-      <c r="T14" s="7">
+      <c r="T14" s="6">
         <v>44418</v>
       </c>
-      <c r="U14" s="7"/>
-      <c r="V14" s="7"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="7"/>
-      <c r="Y14" s="6"/>
-      <c r="Z14" s="6"/>
-      <c r="AA14" s="6"/>
-      <c r="AB14" s="6"/>
-      <c r="AC14" s="6"/>
-      <c r="AD14" s="7"/>
+      <c r="U14" s="6"/>
+      <c r="V14" s="6"/>
+      <c r="W14" s="6"/>
+      <c r="X14" s="6"/>
+      <c r="Y14" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC14" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD14" s="6"/>
       <c r="AE14" s="5" t="s">
         <v>55</v>
       </c>
@@ -2330,17 +2542,19 @@
       <c r="AH14" s="5"/>
       <c r="AI14" s="5"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B15" s="8">
+      <c r="B15" s="7">
         <v>44362</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <v>44722</v>
       </c>
-      <c r="D15" s="6"/>
+      <c r="D15" s="3">
+        <v>0</v>
+      </c>
       <c r="E15" s="5">
         <v>45</v>
       </c>
@@ -2366,31 +2580,47 @@
         <v>1</v>
       </c>
       <c r="M15" s="5"/>
-      <c r="N15" s="5"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="5"/>
-      <c r="Q15" s="9">
+      <c r="N15">
+        <v>0.9</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>1.4</v>
+      </c>
+      <c r="Q15" s="8">
         <v>-82.305835000000002</v>
       </c>
-      <c r="R15" s="9">
+      <c r="R15" s="8">
         <v>37.293075999999999</v>
       </c>
-      <c r="S15" s="7">
+      <c r="S15" s="6">
         <v>44378</v>
       </c>
-      <c r="T15" s="7">
+      <c r="T15" s="6">
         <v>44418</v>
       </c>
-      <c r="U15" s="7"/>
-      <c r="V15" s="7"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="7"/>
-      <c r="Y15" s="6"/>
-      <c r="Z15" s="6"/>
-      <c r="AA15" s="6"/>
-      <c r="AB15" s="6"/>
-      <c r="AC15" s="6"/>
-      <c r="AD15" s="7"/>
+      <c r="U15" s="6"/>
+      <c r="V15" s="6"/>
+      <c r="W15" s="6"/>
+      <c r="X15" s="6"/>
+      <c r="Y15" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC15" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD15" s="6"/>
       <c r="AE15" s="5" t="s">
         <v>55</v>
       </c>
@@ -2401,17 +2631,19 @@
       <c r="AH15" s="5"/>
       <c r="AI15" s="5"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="B16" s="8">
+      <c r="B16" s="7">
         <v>44362</v>
       </c>
-      <c r="C16" s="8">
+      <c r="C16" s="7">
         <v>44682</v>
       </c>
-      <c r="D16" s="6"/>
+      <c r="D16" s="3">
+        <v>0</v>
+      </c>
       <c r="E16" s="5">
         <v>45</v>
       </c>
@@ -2437,31 +2669,47 @@
         <v>1</v>
       </c>
       <c r="M16" s="5"/>
-      <c r="N16" s="5"/>
-      <c r="O16" s="6"/>
-      <c r="P16" s="5"/>
-      <c r="Q16" s="9">
+      <c r="N16">
+        <v>0.9</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>1.4</v>
+      </c>
+      <c r="Q16" s="8">
         <v>-90.958820000000003</v>
       </c>
-      <c r="R16" s="9">
+      <c r="R16" s="8">
         <v>30.657959999999999</v>
       </c>
-      <c r="S16" s="7">
+      <c r="S16" s="6">
         <v>44363</v>
       </c>
-      <c r="T16" s="7">
+      <c r="T16" s="6">
         <v>44418</v>
       </c>
-      <c r="U16" s="7"/>
-      <c r="V16" s="7"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="7"/>
-      <c r="Y16" s="6"/>
-      <c r="Z16" s="6"/>
-      <c r="AA16" s="6"/>
-      <c r="AB16" s="6"/>
-      <c r="AC16" s="6"/>
-      <c r="AD16" s="7"/>
+      <c r="U16" s="6"/>
+      <c r="V16" s="6"/>
+      <c r="W16" s="6"/>
+      <c r="X16" s="6"/>
+      <c r="Y16" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z16" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC16" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD16" s="6"/>
       <c r="AE16" s="5" t="s">
         <v>55</v>
       </c>
@@ -2472,17 +2720,19 @@
       <c r="AH16" s="5"/>
       <c r="AI16" s="5"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="B17" s="8">
+      <c r="B17" s="7">
         <v>44362</v>
       </c>
-      <c r="C17" s="8">
+      <c r="C17" s="7">
         <v>44666</v>
       </c>
-      <c r="D17" s="6"/>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
       <c r="E17" s="5">
         <v>45</v>
       </c>
@@ -2508,31 +2758,47 @@
         <v>1</v>
       </c>
       <c r="M17" s="5"/>
-      <c r="N17" s="5"/>
-      <c r="O17" s="6"/>
-      <c r="P17" s="5"/>
-      <c r="Q17" s="9">
+      <c r="N17">
+        <v>0.9</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>1.4</v>
+      </c>
+      <c r="Q17" s="8">
         <v>30.473739999999999</v>
       </c>
-      <c r="R17" s="9">
+      <c r="R17" s="8">
         <v>-90.992949999999993</v>
       </c>
-      <c r="S17" s="7">
+      <c r="S17" s="6">
         <v>44363</v>
       </c>
-      <c r="T17" s="7">
+      <c r="T17" s="6">
         <v>44418</v>
       </c>
-      <c r="U17" s="7"/>
-      <c r="V17" s="7"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="7"/>
-      <c r="Y17" s="6"/>
-      <c r="Z17" s="6"/>
-      <c r="AA17" s="6"/>
-      <c r="AB17" s="6"/>
-      <c r="AC17" s="6"/>
-      <c r="AD17" s="7"/>
+      <c r="U17" s="6"/>
+      <c r="V17" s="6"/>
+      <c r="W17" s="6"/>
+      <c r="X17" s="6"/>
+      <c r="Y17" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z17" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC17" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD17" s="6"/>
       <c r="AE17" s="5" t="s">
         <v>55</v>
       </c>
@@ -2543,17 +2809,19 @@
       <c r="AH17" s="5"/>
       <c r="AI17" s="5"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="B18" s="8">
+      <c r="B18" s="7">
         <v>44362</v>
       </c>
-      <c r="C18" s="8">
+      <c r="C18" s="7">
         <v>44677</v>
       </c>
-      <c r="D18" s="6"/>
+      <c r="D18" s="3">
+        <v>0</v>
+      </c>
       <c r="E18" s="5">
         <v>45</v>
       </c>
@@ -2579,31 +2847,47 @@
         <v>1</v>
       </c>
       <c r="M18" s="5"/>
-      <c r="N18" s="5"/>
-      <c r="O18" s="6"/>
-      <c r="P18" s="5"/>
-      <c r="Q18" s="9">
+      <c r="N18">
+        <v>0.9</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>1.4</v>
+      </c>
+      <c r="Q18" s="8">
         <v>-91.364180000000005</v>
       </c>
-      <c r="R18" s="9">
+      <c r="R18" s="8">
         <v>30.418990000000001</v>
       </c>
-      <c r="S18" s="7">
+      <c r="S18" s="6">
         <v>44349</v>
       </c>
-      <c r="T18" s="7">
+      <c r="T18" s="6">
         <v>44418</v>
       </c>
-      <c r="U18" s="7"/>
-      <c r="V18" s="7"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="7"/>
-      <c r="Y18" s="6"/>
-      <c r="Z18" s="6"/>
-      <c r="AA18" s="6"/>
-      <c r="AB18" s="6"/>
-      <c r="AC18" s="6"/>
-      <c r="AD18" s="7"/>
+      <c r="U18" s="6"/>
+      <c r="V18" s="6"/>
+      <c r="W18" s="6"/>
+      <c r="X18" s="6"/>
+      <c r="Y18" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z18" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC18" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD18" s="6"/>
       <c r="AE18" s="5" t="s">
         <v>55</v>
       </c>
@@ -2614,17 +2898,19 @@
       <c r="AH18" s="5"/>
       <c r="AI18" s="5"/>
     </row>
-    <row r="19" spans="1:35" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:35" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="B19" s="8">
+      <c r="B19" s="7">
         <v>44362</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="7">
         <v>44684</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="3">
+        <v>0</v>
+      </c>
       <c r="E19" s="5">
         <v>45</v>
       </c>
@@ -2650,31 +2936,47 @@
         <v>1</v>
       </c>
       <c r="M19" s="5"/>
-      <c r="N19" s="5"/>
-      <c r="O19" s="6"/>
-      <c r="P19" s="5"/>
-      <c r="Q19" s="9">
+      <c r="N19">
+        <v>0.9</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>1.4</v>
+      </c>
+      <c r="Q19" s="8">
         <v>-91.371089999999995</v>
       </c>
-      <c r="R19" s="9">
+      <c r="R19" s="8">
         <v>30.415649999999999</v>
       </c>
-      <c r="S19" s="7">
+      <c r="S19" s="6">
         <v>44343</v>
       </c>
-      <c r="T19" s="7">
+      <c r="T19" s="6">
         <v>44418</v>
       </c>
-      <c r="U19" s="7"/>
-      <c r="V19" s="7"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="7"/>
-      <c r="Y19" s="6"/>
-      <c r="Z19" s="6"/>
-      <c r="AA19" s="6"/>
-      <c r="AB19" s="6"/>
-      <c r="AC19" s="6"/>
-      <c r="AD19" s="7"/>
+      <c r="U19" s="6"/>
+      <c r="V19" s="6"/>
+      <c r="W19" s="6"/>
+      <c r="X19" s="6"/>
+      <c r="Y19" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>120</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>100</v>
+      </c>
+      <c r="AC19" s="3">
+        <v>15</v>
+      </c>
+      <c r="AD19" s="6"/>
       <c r="AE19" s="5" t="s">
         <v>55</v>
       </c>

</xml_diff>

<commit_message>
Updated gpr calib settings
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett Rhyne\Documents\SWWA_Connectivity\Analysis\SWWA_Pressure\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8825A549-AD1F-4719-A57A-8AC9FE8290A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0CC6D4-4867-48F8-8BF2-E2487F93589E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="1140" windowWidth="14960" windowHeight="7580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30330" yWindow="3810" windowWidth="22440" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tracks" sheetId="1" r:id="rId1"/>
@@ -202,7 +202,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -360,6 +360,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -717,7 +723,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -731,6 +737,7 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -782,7 +789,10 @@
       <numFmt numFmtId="164" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -797,10 +807,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m/d/yy"/>
@@ -919,14 +926,14 @@
     <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="10"/>
     <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="9"/>
     <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="8"/>
-    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="7"/>
-    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="5"/>
-    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="4"/>
-    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="3"/>
-    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="2"/>
-    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="1"/>
-    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="0"/>
+    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="1"/>
+    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="7"/>
+    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="5"/>
+    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="3"/>
+    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="2"/>
     <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name"/>
     <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name"/>
     <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass"/>
@@ -1237,7 +1244,7 @@
   <dimension ref="A1:AI18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1256,8 +1263,8 @@
     <col min="15" max="16" width="18" customWidth="1"/>
     <col min="17" max="17" width="15.1640625" style="6" customWidth="1"/>
     <col min="18" max="18" width="18.83203125" style="6" customWidth="1"/>
-    <col min="19" max="19" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.33203125" customWidth="1"/>
+    <col min="20" max="20" width="15.33203125" customWidth="1"/>
     <col min="21" max="21" width="15.1640625" customWidth="1"/>
     <col min="22" max="22" width="14.1640625" customWidth="1"/>
     <col min="23" max="25" width="17.33203125" customWidth="1"/>
@@ -1438,12 +1445,20 @@
         <v>44363</v>
       </c>
       <c r="T2" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U2" s="4">
+        <v>44657</v>
+      </c>
+      <c r="V2" s="4">
+        <v>44702</v>
+      </c>
+      <c r="W2" s="6">
+        <v>-80.447980000000001</v>
+      </c>
+      <c r="X2" s="7">
+        <v>32.768059999999998</v>
+      </c>
       <c r="Y2" s="1">
         <v>0.1</v>
       </c>
@@ -1527,12 +1542,20 @@
         <v>44363</v>
       </c>
       <c r="T3" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U3" s="4">
+        <v>44657</v>
+      </c>
+      <c r="V3" s="4">
+        <v>44671</v>
+      </c>
+      <c r="W3" s="7">
+        <v>-80.354759999999999</v>
+      </c>
+      <c r="X3" s="6">
+        <v>33.219625999999998</v>
+      </c>
       <c r="Y3" s="1">
         <v>0.1</v>
       </c>
@@ -1616,12 +1639,20 @@
         <v>44363</v>
       </c>
       <c r="T4" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U4" s="4">
+        <v>44666</v>
+      </c>
+      <c r="V4" s="4">
+        <v>44721</v>
+      </c>
+      <c r="W4" s="8">
+        <v>-84.179299999999998</v>
+      </c>
+      <c r="X4" s="8">
+        <v>35.285809999999998</v>
+      </c>
       <c r="Y4" s="1">
         <v>0.1</v>
       </c>
@@ -1705,12 +1736,20 @@
         <v>44363</v>
       </c>
       <c r="T5" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U5" s="4"/>
-      <c r="V5" s="4"/>
-      <c r="W5" s="4"/>
-      <c r="X5" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U5" s="4">
+        <v>44666</v>
+      </c>
+      <c r="V5" s="4">
+        <v>44697</v>
+      </c>
+      <c r="W5" s="8">
+        <v>-84.049199999999999</v>
+      </c>
+      <c r="X5" s="8">
+        <v>35.439259999999997</v>
+      </c>
       <c r="Y5" s="1">
         <v>0.1</v>
       </c>
@@ -1794,12 +1833,20 @@
         <v>44363</v>
       </c>
       <c r="T6" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U6" s="4"/>
-      <c r="V6" s="4"/>
-      <c r="W6" s="4"/>
-      <c r="X6" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U6" s="4">
+        <v>44666</v>
+      </c>
+      <c r="V6" s="4">
+        <v>44716</v>
+      </c>
+      <c r="W6" s="8">
+        <v>-84.049199999999999</v>
+      </c>
+      <c r="X6" s="8">
+        <v>35.439259999999997</v>
+      </c>
       <c r="Y6" s="1">
         <v>0.1</v>
       </c>
@@ -1883,12 +1930,20 @@
         <v>44363</v>
       </c>
       <c r="T7" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U7" s="4"/>
-      <c r="V7" s="4"/>
-      <c r="W7" s="4"/>
-      <c r="X7" s="4"/>
+        <v>44444</v>
+      </c>
+      <c r="U7" s="4">
+        <v>44666</v>
+      </c>
+      <c r="V7" s="4">
+        <v>44724</v>
+      </c>
+      <c r="W7" s="6">
+        <v>-82.48312</v>
+      </c>
+      <c r="X7" s="6">
+        <v>37.218330000000002</v>
+      </c>
       <c r="Y7" s="1">
         <v>0.1</v>
       </c>
@@ -1972,12 +2027,20 @@
         <v>44363</v>
       </c>
       <c r="T8" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U8" s="4"/>
-      <c r="V8" s="4"/>
-      <c r="W8" s="4"/>
-      <c r="X8" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U8" s="4">
+        <v>44661</v>
+      </c>
+      <c r="V8" s="4">
+        <v>44684</v>
+      </c>
+      <c r="W8" s="6">
+        <v>-91.196119999999993</v>
+      </c>
+      <c r="X8" s="6">
+        <v>36.663780000000003</v>
+      </c>
       <c r="Y8" s="1">
         <v>0.1</v>
       </c>
@@ -2061,12 +2124,20 @@
         <v>44363</v>
       </c>
       <c r="T9" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U9" s="4"/>
-      <c r="V9" s="4"/>
-      <c r="W9" s="4"/>
-      <c r="X9" s="4"/>
+        <v>44444</v>
+      </c>
+      <c r="U9" s="4">
+        <v>44655</v>
+      </c>
+      <c r="V9" s="4">
+        <v>44724</v>
+      </c>
+      <c r="W9" s="6">
+        <v>-82.479211000000006</v>
+      </c>
+      <c r="X9" s="6">
+        <v>37.215834999999998</v>
+      </c>
       <c r="Y9" s="1">
         <v>0.1</v>
       </c>
@@ -2150,12 +2221,20 @@
         <v>44363</v>
       </c>
       <c r="T10" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U10" s="4"/>
-      <c r="V10" s="4"/>
-      <c r="W10" s="4"/>
-      <c r="X10" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U10" s="4">
+        <v>44676</v>
+      </c>
+      <c r="V10" s="4">
+        <v>44684</v>
+      </c>
+      <c r="W10" s="6">
+        <v>-91.197329999999994</v>
+      </c>
+      <c r="X10" s="6">
+        <v>36.650010000000002</v>
+      </c>
       <c r="Y10" s="1">
         <v>0.1</v>
       </c>
@@ -2239,12 +2318,20 @@
         <v>44363</v>
       </c>
       <c r="T11" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U11" s="4">
+        <v>44666</v>
+      </c>
+      <c r="V11" s="4">
+        <v>44685</v>
+      </c>
+      <c r="W11" s="6">
+        <v>-91.214569999999995</v>
+      </c>
+      <c r="X11" s="6">
+        <v>36.732098999999998</v>
+      </c>
       <c r="Y11" s="1">
         <v>0.1</v>
       </c>
@@ -2328,12 +2415,20 @@
         <v>44378</v>
       </c>
       <c r="T12" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U12" s="4"/>
-      <c r="V12" s="4"/>
-      <c r="W12" s="4"/>
-      <c r="X12" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U12" s="4">
+        <v>44671</v>
+      </c>
+      <c r="V12" s="4">
+        <v>44726</v>
+      </c>
+      <c r="W12" s="6">
+        <v>-82.301767999999996</v>
+      </c>
+      <c r="X12" s="6">
+        <v>37.294294999999998</v>
+      </c>
       <c r="Y12" s="1">
         <v>0.1</v>
       </c>
@@ -2417,12 +2512,20 @@
         <v>44378</v>
       </c>
       <c r="T13" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U13" s="4"/>
-      <c r="V13" s="4"/>
-      <c r="W13" s="4"/>
-      <c r="X13" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U13" s="4">
+        <v>44671</v>
+      </c>
+      <c r="V13" s="4">
+        <v>44722</v>
+      </c>
+      <c r="W13" s="6">
+        <v>-82.304972000000006</v>
+      </c>
+      <c r="X13" s="6">
+        <v>37.286811999999998</v>
+      </c>
       <c r="Y13" s="1">
         <v>0.1</v>
       </c>
@@ -2506,12 +2609,20 @@
         <v>44378</v>
       </c>
       <c r="T14" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U14" s="4">
+        <v>44676</v>
+      </c>
+      <c r="V14" s="4">
+        <v>44722</v>
+      </c>
+      <c r="W14" s="6">
+        <v>-82.305835000000002</v>
+      </c>
+      <c r="X14" s="6">
+        <v>37.293075999999999</v>
+      </c>
       <c r="Y14" s="1">
         <v>0.1</v>
       </c>
@@ -2595,12 +2706,20 @@
         <v>44363</v>
       </c>
       <c r="T15" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U15" s="4"/>
-      <c r="V15" s="4"/>
-      <c r="W15" s="4"/>
-      <c r="X15" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U15" s="4">
+        <v>44662</v>
+      </c>
+      <c r="V15" s="9">
+        <v>44682</v>
+      </c>
+      <c r="W15" s="6">
+        <v>-90.958820000000003</v>
+      </c>
+      <c r="X15" s="6">
+        <v>30.657959999999999</v>
+      </c>
       <c r="Y15" s="1">
         <v>0.1</v>
       </c>
@@ -2684,12 +2803,20 @@
         <v>44363</v>
       </c>
       <c r="T16" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U16" s="4"/>
-      <c r="V16" s="4"/>
-      <c r="W16" s="4"/>
-      <c r="X16" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U16" s="4">
+        <v>44652</v>
+      </c>
+      <c r="V16" s="9">
+        <v>44666</v>
+      </c>
+      <c r="W16" s="6">
+        <v>30.473739999999999</v>
+      </c>
+      <c r="X16" s="6">
+        <v>-90.992949999999993</v>
+      </c>
       <c r="Y16" s="1">
         <v>0.1</v>
       </c>
@@ -2773,12 +2900,20 @@
         <v>44349</v>
       </c>
       <c r="T17" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U17" s="4"/>
-      <c r="V17" s="4"/>
-      <c r="W17" s="4"/>
-      <c r="X17" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U17" s="4">
+        <v>44655</v>
+      </c>
+      <c r="V17" s="9">
+        <v>44677</v>
+      </c>
+      <c r="W17" s="6">
+        <v>-91.364180000000005</v>
+      </c>
+      <c r="X17" s="6">
+        <v>30.418990000000001</v>
+      </c>
       <c r="Y17" s="1">
         <v>0.1</v>
       </c>
@@ -2862,12 +2997,20 @@
         <v>44343</v>
       </c>
       <c r="T18" s="4">
-        <v>44418</v>
-      </c>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
+        <v>44454</v>
+      </c>
+      <c r="U18" s="4">
+        <v>44659</v>
+      </c>
+      <c r="V18" s="9">
+        <v>44684</v>
+      </c>
+      <c r="W18" s="6">
+        <v>-91.371089999999995</v>
+      </c>
+      <c r="X18" s="6">
+        <v>30.415649999999999</v>
+      </c>
       <c r="Y18" s="1">
         <v>0.1</v>
       </c>

</xml_diff>

<commit_message>
Tag data commit (Sep 5)
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett Rhyne\Documents\SWWA_Connectivity\Analysis\SWWA_Pressure\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E0CC6D4-4867-48F8-8BF2-E2487F93589E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599D2EAB-7BDA-4512-84AE-9E355182E837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="30330" yWindow="3810" windowWidth="22440" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -723,20 +723,17 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="42" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="22" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
@@ -789,10 +786,7 @@
       <numFmt numFmtId="164" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yy"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -807,7 +801,10 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="m/d/yy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="m/d/yy"/>
@@ -926,14 +923,14 @@
     <tableColumn id="20" xr3:uid="{F0057B32-84F6-0D4E-B0D3-B8591BCF0A33}" name="calib_1_end" dataDxfId="10"/>
     <tableColumn id="21" xr3:uid="{72C1CC5C-0A2A-3140-9A33-1BAC20CBDE1B}" name="calib_2_start" dataDxfId="9"/>
     <tableColumn id="22" xr3:uid="{1E9B142A-92EB-D647-BB56-ADFB8F3B1DE9}" name="calib_2_end" dataDxfId="8"/>
-    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="1"/>
-    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="7"/>
-    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="5"/>
-    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="3"/>
-    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="2"/>
+    <tableColumn id="40" xr3:uid="{ABB1AA27-3007-954E-BFD9-D15B5759E520}" name="calib_2_lon" dataDxfId="7"/>
+    <tableColumn id="41" xr3:uid="{5A6DF468-93CA-8E49-B529-24F965EC5A68}" name="calib_2_lat" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C1C8E7B8-04FB-6241-9466-61A298BC202A}" name="prob_light_w" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{CA9C149A-C070-ED44-9095-795932D8BA41}" name="thr_prob_percentile" dataDxfId="4"/>
+    <tableColumn id="7" xr3:uid="{74B13C9B-EDD7-A24E-A7E5-146255BCE559}" name="thr_gs" dataDxfId="3"/>
+    <tableColumn id="13" xr3:uid="{07BAD23C-A227-CE4D-A5DA-81F573B31782}" name="thr_as" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{4C9C4E26-983D-354E-9081-3E245F2F2396}" name="low_speed_fix" dataDxfId="1"/>
+    <tableColumn id="32" xr3:uid="{8FB298A1-7B27-ED49-9E23-106210114304}" name="ringNo" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{437D6807-140D-EC48-A588-9CA0C70671A6}" name="scientific_name"/>
     <tableColumn id="5" xr3:uid="{E0EF373A-0600-B64D-81CD-63E6714931D7}" name="common_name"/>
     <tableColumn id="34" xr3:uid="{AAB4E28F-C2D5-A44D-A5CF-C6EA295E6EC5}" name="mass"/>
@@ -1244,7 +1241,7 @@
   <dimension ref="A1:AI18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1261,8 +1258,8 @@
     <col min="13" max="13" width="21.33203125" customWidth="1"/>
     <col min="14" max="14" width="18.75" customWidth="1"/>
     <col min="15" max="16" width="18" customWidth="1"/>
-    <col min="17" max="17" width="15.1640625" style="6" customWidth="1"/>
-    <col min="18" max="18" width="18.83203125" style="6" customWidth="1"/>
+    <col min="17" max="17" width="15.1640625" customWidth="1"/>
+    <col min="18" max="18" width="18.83203125" customWidth="1"/>
     <col min="19" max="19" width="14.33203125" customWidth="1"/>
     <col min="20" max="20" width="15.33203125" customWidth="1"/>
     <col min="21" max="21" width="15.1640625" customWidth="1"/>
@@ -1330,10 +1327,10 @@
       <c r="P1" t="s">
         <v>29</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="Q1" t="s">
         <v>6</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="R1" t="s">
         <v>7</v>
       </c>
       <c r="S1" t="s">
@@ -1389,43 +1386,42 @@
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="5">
+      <c r="B2" s="3">
         <v>44362</v>
       </c>
-      <c r="C2" s="5">
+      <c r="C2" s="3">
         <v>44702</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2">
         <v>12</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>45</v>
       </c>
-      <c r="F2" s="3">
+      <c r="F2">
         <v>-97</v>
       </c>
-      <c r="G2" s="3">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3">
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
         <v>-71</v>
       </c>
-      <c r="I2" s="3">
+      <c r="I2">
         <v>5</v>
       </c>
-      <c r="J2" s="3">
+      <c r="J2">
         <v>300</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2">
         <v>30</v>
       </c>
-      <c r="L2" s="3">
+      <c r="L2">
         <v>1</v>
       </c>
-      <c r="M2" s="3"/>
       <c r="N2">
         <v>0.9</v>
       </c>
@@ -1435,94 +1431,90 @@
       <c r="P2">
         <v>1.4</v>
       </c>
-      <c r="Q2" s="6">
+      <c r="Q2">
         <v>-80.447980000000001</v>
       </c>
-      <c r="R2" s="7">
+      <c r="R2" s="4">
         <v>32.768059999999998</v>
       </c>
-      <c r="S2" s="4">
+      <c r="S2" s="2">
         <v>44363</v>
       </c>
-      <c r="T2" s="4">
+      <c r="T2" s="2">
         <v>44454</v>
       </c>
-      <c r="U2" s="4">
+      <c r="U2" s="2">
         <v>44657</v>
       </c>
-      <c r="V2" s="4">
+      <c r="V2" s="2">
         <v>44702</v>
       </c>
-      <c r="W2" s="6">
+      <c r="W2">
         <v>-80.447980000000001</v>
       </c>
-      <c r="X2" s="7">
+      <c r="X2" s="4">
         <v>32.768059999999998</v>
       </c>
-      <c r="Y2" s="1">
+      <c r="Y2">
         <v>0.1</v>
       </c>
-      <c r="Z2" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA2" s="1">
+      <c r="Z2">
+        <v>0.9</v>
+      </c>
+      <c r="AA2">
         <v>120</v>
       </c>
-      <c r="AB2" s="1">
+      <c r="AB2">
         <v>100</v>
       </c>
-      <c r="AC2" s="1">
+      <c r="AC2">
         <v>15</v>
       </c>
-      <c r="AD2" s="4"/>
-      <c r="AE2" s="3" t="s">
+      <c r="AD2" s="2"/>
+      <c r="AE2" t="s">
         <v>52</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AF2" t="s">
         <v>53</v>
       </c>
-      <c r="AG2" s="3"/>
-      <c r="AH2" s="3"/>
-      <c r="AI2" s="3"/>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="5">
+      <c r="B3" s="3">
         <v>44362</v>
       </c>
-      <c r="C3" s="5">
+      <c r="C3" s="3">
         <v>44671</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3">
         <v>12</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3">
         <v>45</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3">
         <v>-97</v>
       </c>
-      <c r="G3" s="3">
-        <v>0</v>
-      </c>
-      <c r="H3" s="3">
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
         <v>-71</v>
       </c>
-      <c r="I3" s="3">
+      <c r="I3">
         <v>5</v>
       </c>
-      <c r="J3" s="3">
+      <c r="J3">
         <v>300</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3">
         <v>30</v>
       </c>
-      <c r="L3" s="3">
+      <c r="L3">
         <v>1</v>
       </c>
-      <c r="M3" s="3"/>
       <c r="N3">
         <v>0.9</v>
       </c>
@@ -1532,94 +1524,90 @@
       <c r="P3">
         <v>1.4</v>
       </c>
-      <c r="Q3" s="7">
+      <c r="Q3" s="4">
         <v>-80.354759999999999</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3">
         <v>33.219625999999998</v>
       </c>
-      <c r="S3" s="4">
+      <c r="S3" s="2">
         <v>44363</v>
       </c>
-      <c r="T3" s="4">
+      <c r="T3" s="2">
         <v>44454</v>
       </c>
-      <c r="U3" s="4">
+      <c r="U3" s="2">
         <v>44657</v>
       </c>
-      <c r="V3" s="4">
+      <c r="V3" s="2">
         <v>44671</v>
       </c>
-      <c r="W3" s="7">
+      <c r="W3" s="4">
         <v>-80.354759999999999</v>
       </c>
-      <c r="X3" s="6">
+      <c r="X3">
         <v>33.219625999999998</v>
       </c>
-      <c r="Y3" s="1">
+      <c r="Y3">
         <v>0.1</v>
       </c>
-      <c r="Z3" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA3" s="1">
+      <c r="Z3">
+        <v>0.9</v>
+      </c>
+      <c r="AA3">
         <v>120</v>
       </c>
-      <c r="AB3" s="1">
+      <c r="AB3">
         <v>100</v>
       </c>
-      <c r="AC3" s="1">
+      <c r="AC3">
         <v>15</v>
       </c>
-      <c r="AD3" s="4"/>
-      <c r="AE3" s="3" t="s">
+      <c r="AD3" s="2"/>
+      <c r="AE3" t="s">
         <v>52</v>
       </c>
-      <c r="AF3" s="3" t="s">
+      <c r="AF3" t="s">
         <v>53</v>
       </c>
-      <c r="AG3" s="3"/>
-      <c r="AH3" s="3"/>
-      <c r="AI3" s="3"/>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>44362</v>
       </c>
-      <c r="C4" s="5">
+      <c r="C4" s="3">
         <v>44721</v>
       </c>
-      <c r="D4" s="1">
-        <v>12</v>
-      </c>
-      <c r="E4" s="3">
+      <c r="D4">
+        <v>24</v>
+      </c>
+      <c r="E4">
         <v>45</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4">
         <v>-97</v>
       </c>
-      <c r="G4" s="3">
-        <v>0</v>
-      </c>
-      <c r="H4" s="3">
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
         <v>-71</v>
       </c>
-      <c r="I4" s="3">
+      <c r="I4">
         <v>5</v>
       </c>
-      <c r="J4" s="3">
+      <c r="J4">
         <v>300</v>
       </c>
-      <c r="K4" s="3">
+      <c r="K4">
         <v>30</v>
       </c>
-      <c r="L4" s="3">
+      <c r="L4">
         <v>1</v>
       </c>
-      <c r="M4" s="3"/>
       <c r="N4">
         <v>0.9</v>
       </c>
@@ -1629,94 +1617,90 @@
       <c r="P4">
         <v>1.4</v>
       </c>
-      <c r="Q4" s="8">
+      <c r="Q4" s="5">
         <v>-84.179299999999998</v>
       </c>
-      <c r="R4" s="8">
+      <c r="R4" s="5">
         <v>35.285809999999998</v>
       </c>
-      <c r="S4" s="4">
+      <c r="S4" s="2">
         <v>44363</v>
       </c>
-      <c r="T4" s="4">
+      <c r="T4" s="2">
         <v>44454</v>
       </c>
-      <c r="U4" s="4">
+      <c r="U4" s="2">
         <v>44666</v>
       </c>
-      <c r="V4" s="4">
+      <c r="V4" s="2">
         <v>44721</v>
       </c>
-      <c r="W4" s="8">
+      <c r="W4" s="5">
         <v>-84.179299999999998</v>
       </c>
-      <c r="X4" s="8">
+      <c r="X4" s="5">
         <v>35.285809999999998</v>
       </c>
-      <c r="Y4" s="1">
+      <c r="Y4">
         <v>0.1</v>
       </c>
-      <c r="Z4" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA4" s="1">
+      <c r="Z4">
+        <v>0.9</v>
+      </c>
+      <c r="AA4">
         <v>120</v>
       </c>
-      <c r="AB4" s="1">
+      <c r="AB4">
         <v>100</v>
       </c>
-      <c r="AC4" s="1">
+      <c r="AC4">
         <v>15</v>
       </c>
-      <c r="AD4" s="4"/>
-      <c r="AE4" s="3" t="s">
+      <c r="AD4" s="2"/>
+      <c r="AE4" t="s">
         <v>52</v>
       </c>
-      <c r="AF4" s="3" t="s">
+      <c r="AF4" t="s">
         <v>53</v>
       </c>
-      <c r="AG4" s="3"/>
-      <c r="AH4" s="3"/>
-      <c r="AI4" s="3"/>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="3">
         <v>44362</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="3">
         <v>44697</v>
       </c>
-      <c r="D5" s="1">
+      <c r="D5">
         <v>12</v>
       </c>
-      <c r="E5" s="3">
+      <c r="E5">
         <v>45</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5">
         <v>-97</v>
       </c>
-      <c r="G5" s="3">
-        <v>0</v>
-      </c>
-      <c r="H5" s="3">
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
         <v>-71</v>
       </c>
-      <c r="I5" s="3">
+      <c r="I5">
         <v>5</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5">
         <v>300</v>
       </c>
-      <c r="K5" s="3">
+      <c r="K5">
         <v>30</v>
       </c>
-      <c r="L5" s="3">
+      <c r="L5">
         <v>1</v>
       </c>
-      <c r="M5" s="3"/>
       <c r="N5">
         <v>0.9</v>
       </c>
@@ -1726,94 +1710,90 @@
       <c r="P5">
         <v>1.4</v>
       </c>
-      <c r="Q5" s="8">
+      <c r="Q5" s="5">
         <v>-84.049199999999999</v>
       </c>
-      <c r="R5" s="8">
+      <c r="R5" s="5">
         <v>35.439259999999997</v>
       </c>
-      <c r="S5" s="4">
+      <c r="S5" s="2">
         <v>44363</v>
       </c>
-      <c r="T5" s="4">
+      <c r="T5" s="2">
         <v>44454</v>
       </c>
-      <c r="U5" s="4">
+      <c r="U5" s="2">
         <v>44666</v>
       </c>
-      <c r="V5" s="4">
+      <c r="V5" s="2">
         <v>44697</v>
       </c>
-      <c r="W5" s="8">
+      <c r="W5" s="5">
         <v>-84.049199999999999</v>
       </c>
-      <c r="X5" s="8">
+      <c r="X5" s="5">
         <v>35.439259999999997</v>
       </c>
-      <c r="Y5" s="1">
+      <c r="Y5">
         <v>0.1</v>
       </c>
-      <c r="Z5" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA5" s="1">
+      <c r="Z5">
+        <v>0.9</v>
+      </c>
+      <c r="AA5">
         <v>120</v>
       </c>
-      <c r="AB5" s="1">
+      <c r="AB5">
         <v>100</v>
       </c>
-      <c r="AC5" s="1">
+      <c r="AC5">
         <v>15</v>
       </c>
-      <c r="AD5" s="4"/>
-      <c r="AE5" s="3" t="s">
+      <c r="AD5" s="2"/>
+      <c r="AE5" t="s">
         <v>52</v>
       </c>
-      <c r="AF5" s="3" t="s">
+      <c r="AF5" t="s">
         <v>53</v>
       </c>
-      <c r="AG5" s="3"/>
-      <c r="AH5" s="3"/>
-      <c r="AI5" s="3"/>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B6" s="5">
+      <c r="B6" s="3">
         <v>44362</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="3">
         <v>44716</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6">
         <v>12</v>
       </c>
-      <c r="E6" s="3">
+      <c r="E6">
         <v>45</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6">
         <v>-97</v>
       </c>
-      <c r="G6" s="3">
-        <v>0</v>
-      </c>
-      <c r="H6" s="3">
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
         <v>-71</v>
       </c>
-      <c r="I6" s="3">
+      <c r="I6">
         <v>5</v>
       </c>
-      <c r="J6" s="3">
+      <c r="J6">
         <v>300</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6">
         <v>30</v>
       </c>
-      <c r="L6" s="3">
+      <c r="L6">
         <v>1</v>
       </c>
-      <c r="M6" s="3"/>
       <c r="N6">
         <v>0.9</v>
       </c>
@@ -1823,94 +1803,90 @@
       <c r="P6">
         <v>1.4</v>
       </c>
-      <c r="Q6" s="8">
+      <c r="Q6" s="5">
         <v>-84.049199999999999</v>
       </c>
-      <c r="R6" s="8">
+      <c r="R6" s="5">
         <v>35.439259999999997</v>
       </c>
-      <c r="S6" s="4">
+      <c r="S6" s="2">
         <v>44363</v>
       </c>
-      <c r="T6" s="4">
+      <c r="T6" s="2">
         <v>44454</v>
       </c>
-      <c r="U6" s="4">
+      <c r="U6" s="2">
         <v>44666</v>
       </c>
-      <c r="V6" s="4">
+      <c r="V6" s="2">
         <v>44716</v>
       </c>
-      <c r="W6" s="8">
+      <c r="W6" s="5">
         <v>-84.049199999999999</v>
       </c>
-      <c r="X6" s="8">
+      <c r="X6" s="5">
         <v>35.439259999999997</v>
       </c>
-      <c r="Y6" s="1">
+      <c r="Y6">
         <v>0.1</v>
       </c>
-      <c r="Z6" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA6" s="1">
+      <c r="Z6">
+        <v>0.9</v>
+      </c>
+      <c r="AA6">
         <v>120</v>
       </c>
-      <c r="AB6" s="1">
+      <c r="AB6">
         <v>100</v>
       </c>
-      <c r="AC6" s="1">
+      <c r="AC6">
         <v>15</v>
       </c>
-      <c r="AD6" s="4"/>
-      <c r="AE6" s="3" t="s">
+      <c r="AD6" s="2"/>
+      <c r="AE6" t="s">
         <v>52</v>
       </c>
-      <c r="AF6" s="3" t="s">
+      <c r="AF6" t="s">
         <v>53</v>
       </c>
-      <c r="AG6" s="3"/>
-      <c r="AH6" s="3"/>
-      <c r="AI6" s="3"/>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="5">
+      <c r="B7" s="3">
         <v>44370</v>
       </c>
-      <c r="C7" s="5">
+      <c r="C7" s="3">
         <v>44724</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7">
         <v>12</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7">
         <v>45</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7">
         <v>-97</v>
       </c>
-      <c r="G7" s="3">
-        <v>0</v>
-      </c>
-      <c r="H7" s="3">
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
         <v>-71</v>
       </c>
-      <c r="I7" s="3">
+      <c r="I7">
         <v>5</v>
       </c>
-      <c r="J7" s="3">
+      <c r="J7">
         <v>300</v>
       </c>
-      <c r="K7" s="3">
+      <c r="K7">
         <v>30</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7">
         <v>1</v>
       </c>
-      <c r="M7" s="3"/>
       <c r="N7">
         <v>0.9</v>
       </c>
@@ -1920,94 +1896,90 @@
       <c r="P7">
         <v>1.4</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7">
         <v>-82.48312</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7">
         <v>37.218330000000002</v>
       </c>
-      <c r="S7" s="4">
+      <c r="S7" s="2">
         <v>44363</v>
       </c>
-      <c r="T7" s="4">
+      <c r="T7" s="2">
         <v>44444</v>
       </c>
-      <c r="U7" s="4">
+      <c r="U7" s="2">
         <v>44666</v>
       </c>
-      <c r="V7" s="4">
+      <c r="V7" s="2">
         <v>44724</v>
       </c>
-      <c r="W7" s="6">
+      <c r="W7">
         <v>-82.48312</v>
       </c>
-      <c r="X7" s="6">
+      <c r="X7">
         <v>37.218330000000002</v>
       </c>
-      <c r="Y7" s="1">
+      <c r="Y7">
         <v>0.1</v>
       </c>
-      <c r="Z7" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA7" s="1">
+      <c r="Z7">
+        <v>0.9</v>
+      </c>
+      <c r="AA7">
         <v>120</v>
       </c>
-      <c r="AB7" s="1">
+      <c r="AB7">
         <v>100</v>
       </c>
-      <c r="AC7" s="1">
+      <c r="AC7">
         <v>15</v>
       </c>
-      <c r="AD7" s="4"/>
-      <c r="AE7" s="3" t="s">
+      <c r="AD7" s="2"/>
+      <c r="AE7" t="s">
         <v>52</v>
       </c>
-      <c r="AF7" s="3" t="s">
+      <c r="AF7" t="s">
         <v>53</v>
       </c>
-      <c r="AG7" s="3"/>
-      <c r="AH7" s="3"/>
-      <c r="AI7" s="3"/>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="5">
+      <c r="B8" s="3">
         <v>44362</v>
       </c>
-      <c r="C8" s="5">
+      <c r="C8" s="3">
         <v>44684</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8">
         <v>12</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8">
         <v>45</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8">
         <v>-97</v>
       </c>
-      <c r="G8" s="3">
-        <v>0</v>
-      </c>
-      <c r="H8" s="3">
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
         <v>-71</v>
       </c>
-      <c r="I8" s="3">
+      <c r="I8">
         <v>5</v>
       </c>
-      <c r="J8" s="3">
+      <c r="J8">
         <v>300</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8">
         <v>30</v>
       </c>
-      <c r="L8" s="3">
+      <c r="L8">
         <v>1</v>
       </c>
-      <c r="M8" s="3"/>
       <c r="N8">
         <v>0.9</v>
       </c>
@@ -2017,94 +1989,90 @@
       <c r="P8">
         <v>1.4</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8">
         <v>-91.196119999999993</v>
       </c>
-      <c r="R8" s="6">
+      <c r="R8">
         <v>36.663780000000003</v>
       </c>
-      <c r="S8" s="4">
+      <c r="S8" s="2">
         <v>44363</v>
       </c>
-      <c r="T8" s="4">
+      <c r="T8" s="2">
         <v>44454</v>
       </c>
-      <c r="U8" s="4">
+      <c r="U8" s="2">
         <v>44661</v>
       </c>
-      <c r="V8" s="4">
+      <c r="V8" s="2">
         <v>44684</v>
       </c>
-      <c r="W8" s="6">
+      <c r="W8">
         <v>-91.196119999999993</v>
       </c>
-      <c r="X8" s="6">
+      <c r="X8">
         <v>36.663780000000003</v>
       </c>
-      <c r="Y8" s="1">
+      <c r="Y8">
         <v>0.1</v>
       </c>
-      <c r="Z8" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA8" s="1">
+      <c r="Z8">
+        <v>0.9</v>
+      </c>
+      <c r="AA8">
         <v>120</v>
       </c>
-      <c r="AB8" s="1">
+      <c r="AB8">
         <v>100</v>
       </c>
-      <c r="AC8" s="1">
+      <c r="AC8">
         <v>15</v>
       </c>
-      <c r="AD8" s="4"/>
-      <c r="AE8" s="3" t="s">
+      <c r="AD8" s="2"/>
+      <c r="AE8" t="s">
         <v>52</v>
       </c>
-      <c r="AF8" s="3" t="s">
+      <c r="AF8" t="s">
         <v>53</v>
       </c>
-      <c r="AG8" s="3"/>
-      <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="5">
+      <c r="B9" s="3">
         <v>44370</v>
       </c>
-      <c r="C9" s="5">
+      <c r="C9" s="3">
         <v>44724</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9">
         <v>12</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9">
         <v>45</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9">
         <v>-97</v>
       </c>
-      <c r="G9" s="3">
-        <v>0</v>
-      </c>
-      <c r="H9" s="3">
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
         <v>-71</v>
       </c>
-      <c r="I9" s="3">
+      <c r="I9">
         <v>5</v>
       </c>
-      <c r="J9" s="3">
+      <c r="J9">
         <v>300</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9">
         <v>30</v>
       </c>
-      <c r="L9" s="3">
+      <c r="L9">
         <v>1</v>
       </c>
-      <c r="M9" s="3"/>
       <c r="N9">
         <v>0.9</v>
       </c>
@@ -2114,94 +2082,90 @@
       <c r="P9">
         <v>1.4</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9">
         <v>-82.479211000000006</v>
       </c>
-      <c r="R9" s="6">
+      <c r="R9">
         <v>37.215834999999998</v>
       </c>
-      <c r="S9" s="4">
+      <c r="S9" s="2">
         <v>44363</v>
       </c>
-      <c r="T9" s="4">
+      <c r="T9" s="2">
         <v>44444</v>
       </c>
-      <c r="U9" s="4">
+      <c r="U9" s="2">
         <v>44655</v>
       </c>
-      <c r="V9" s="4">
+      <c r="V9" s="2">
         <v>44724</v>
       </c>
-      <c r="W9" s="6">
+      <c r="W9">
         <v>-82.479211000000006</v>
       </c>
-      <c r="X9" s="6">
+      <c r="X9">
         <v>37.215834999999998</v>
       </c>
-      <c r="Y9" s="1">
+      <c r="Y9">
         <v>0.1</v>
       </c>
-      <c r="Z9" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA9" s="1">
+      <c r="Z9">
+        <v>0.9</v>
+      </c>
+      <c r="AA9">
         <v>120</v>
       </c>
-      <c r="AB9" s="1">
+      <c r="AB9">
         <v>100</v>
       </c>
-      <c r="AC9" s="1">
+      <c r="AC9">
         <v>15</v>
       </c>
-      <c r="AD9" s="4"/>
-      <c r="AE9" s="3" t="s">
+      <c r="AD9" s="2"/>
+      <c r="AE9" t="s">
         <v>52</v>
       </c>
-      <c r="AF9" s="3" t="s">
+      <c r="AF9" t="s">
         <v>53</v>
       </c>
-      <c r="AG9" s="3"/>
-      <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="3">
         <v>44362</v>
       </c>
-      <c r="C10" s="5">
+      <c r="C10" s="3">
         <v>44684</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10">
         <v>12</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10">
         <v>45</v>
       </c>
-      <c r="F10" s="3">
+      <c r="F10">
         <v>-97</v>
       </c>
-      <c r="G10" s="3">
-        <v>0</v>
-      </c>
-      <c r="H10" s="3">
+      <c r="G10">
+        <v>0</v>
+      </c>
+      <c r="H10">
         <v>-71</v>
       </c>
-      <c r="I10" s="3">
+      <c r="I10">
         <v>5</v>
       </c>
-      <c r="J10" s="3">
+      <c r="J10">
         <v>300</v>
       </c>
-      <c r="K10" s="3">
+      <c r="K10">
         <v>30</v>
       </c>
-      <c r="L10" s="3">
+      <c r="L10">
         <v>1</v>
       </c>
-      <c r="M10" s="3"/>
       <c r="N10">
         <v>0.9</v>
       </c>
@@ -2211,94 +2175,90 @@
       <c r="P10">
         <v>1.4</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10">
         <v>-91.197329999999994</v>
       </c>
-      <c r="R10" s="6">
+      <c r="R10">
         <v>36.650010000000002</v>
       </c>
-      <c r="S10" s="4">
+      <c r="S10" s="2">
         <v>44363</v>
       </c>
-      <c r="T10" s="4">
+      <c r="T10" s="2">
         <v>44454</v>
       </c>
-      <c r="U10" s="4">
+      <c r="U10" s="2">
         <v>44676</v>
       </c>
-      <c r="V10" s="4">
+      <c r="V10" s="2">
         <v>44684</v>
       </c>
-      <c r="W10" s="6">
+      <c r="W10">
         <v>-91.197329999999994</v>
       </c>
-      <c r="X10" s="6">
+      <c r="X10">
         <v>36.650010000000002</v>
       </c>
-      <c r="Y10" s="1">
+      <c r="Y10">
         <v>0.1</v>
       </c>
-      <c r="Z10" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA10" s="1">
+      <c r="Z10">
+        <v>0.9</v>
+      </c>
+      <c r="AA10">
         <v>120</v>
       </c>
-      <c r="AB10" s="1">
+      <c r="AB10">
         <v>100</v>
       </c>
-      <c r="AC10" s="1">
+      <c r="AC10">
         <v>15</v>
       </c>
-      <c r="AD10" s="4"/>
-      <c r="AE10" s="3" t="s">
+      <c r="AD10" s="2"/>
+      <c r="AE10" t="s">
         <v>52</v>
       </c>
-      <c r="AF10" s="3" t="s">
+      <c r="AF10" t="s">
         <v>53</v>
       </c>
-      <c r="AG10" s="3"/>
-      <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="3">
         <v>44362</v>
       </c>
-      <c r="C11" s="5">
+      <c r="C11" s="3">
         <v>44685</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11">
         <v>12</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11">
         <v>45</v>
       </c>
-      <c r="F11" s="3">
+      <c r="F11">
         <v>-97</v>
       </c>
-      <c r="G11" s="3">
-        <v>0</v>
-      </c>
-      <c r="H11" s="3">
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
         <v>-71</v>
       </c>
-      <c r="I11" s="3">
+      <c r="I11">
         <v>5</v>
       </c>
-      <c r="J11" s="3">
+      <c r="J11">
         <v>300</v>
       </c>
-      <c r="K11" s="3">
+      <c r="K11">
         <v>30</v>
       </c>
-      <c r="L11" s="3">
+      <c r="L11">
         <v>1</v>
       </c>
-      <c r="M11" s="3"/>
       <c r="N11">
         <v>0.9</v>
       </c>
@@ -2308,94 +2268,90 @@
       <c r="P11">
         <v>1.4</v>
       </c>
-      <c r="Q11" s="6">
+      <c r="Q11">
         <v>-91.214569999999995</v>
       </c>
-      <c r="R11" s="6">
+      <c r="R11">
         <v>36.732098999999998</v>
       </c>
-      <c r="S11" s="4">
+      <c r="S11" s="2">
         <v>44363</v>
       </c>
-      <c r="T11" s="4">
+      <c r="T11" s="2">
         <v>44454</v>
       </c>
-      <c r="U11" s="4">
+      <c r="U11" s="2">
         <v>44666</v>
       </c>
-      <c r="V11" s="4">
+      <c r="V11" s="2">
         <v>44685</v>
       </c>
-      <c r="W11" s="6">
+      <c r="W11">
         <v>-91.214569999999995</v>
       </c>
-      <c r="X11" s="6">
+      <c r="X11">
         <v>36.732098999999998</v>
       </c>
-      <c r="Y11" s="1">
+      <c r="Y11">
         <v>0.1</v>
       </c>
-      <c r="Z11" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA11" s="1">
+      <c r="Z11">
+        <v>0.9</v>
+      </c>
+      <c r="AA11">
         <v>120</v>
       </c>
-      <c r="AB11" s="1">
+      <c r="AB11">
         <v>100</v>
       </c>
-      <c r="AC11" s="1">
+      <c r="AC11">
         <v>15</v>
       </c>
-      <c r="AD11" s="4"/>
-      <c r="AE11" s="3" t="s">
+      <c r="AD11" s="2"/>
+      <c r="AE11" t="s">
         <v>52</v>
       </c>
-      <c r="AF11" s="3" t="s">
+      <c r="AF11" t="s">
         <v>53</v>
       </c>
-      <c r="AG11" s="3"/>
-      <c r="AH11" s="3"/>
-      <c r="AI11" s="3"/>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="3">
         <v>44362</v>
       </c>
-      <c r="C12" s="5">
+      <c r="C12" s="3">
         <v>44726</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12">
         <v>12</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12">
         <v>45</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12">
         <v>-97</v>
       </c>
-      <c r="G12" s="3">
-        <v>0</v>
-      </c>
-      <c r="H12" s="3">
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
         <v>-71</v>
       </c>
-      <c r="I12" s="3">
+      <c r="I12">
         <v>5</v>
       </c>
-      <c r="J12" s="3">
+      <c r="J12">
         <v>300</v>
       </c>
-      <c r="K12" s="3">
+      <c r="K12">
         <v>30</v>
       </c>
-      <c r="L12" s="3">
+      <c r="L12">
         <v>1</v>
       </c>
-      <c r="M12" s="3"/>
       <c r="N12">
         <v>0.9</v>
       </c>
@@ -2405,94 +2361,90 @@
       <c r="P12">
         <v>1.4</v>
       </c>
-      <c r="Q12" s="6">
+      <c r="Q12">
         <v>-82.301767999999996</v>
       </c>
-      <c r="R12" s="6">
+      <c r="R12">
         <v>37.294294999999998</v>
       </c>
-      <c r="S12" s="4">
+      <c r="S12" s="2">
         <v>44378</v>
       </c>
-      <c r="T12" s="4">
+      <c r="T12" s="2">
         <v>44454</v>
       </c>
-      <c r="U12" s="4">
+      <c r="U12" s="2">
         <v>44671</v>
       </c>
-      <c r="V12" s="4">
+      <c r="V12" s="2">
         <v>44726</v>
       </c>
-      <c r="W12" s="6">
+      <c r="W12">
         <v>-82.301767999999996</v>
       </c>
-      <c r="X12" s="6">
+      <c r="X12">
         <v>37.294294999999998</v>
       </c>
-      <c r="Y12" s="1">
+      <c r="Y12">
         <v>0.1</v>
       </c>
-      <c r="Z12" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA12" s="1">
+      <c r="Z12">
+        <v>0.9</v>
+      </c>
+      <c r="AA12">
         <v>120</v>
       </c>
-      <c r="AB12" s="1">
+      <c r="AB12">
         <v>100</v>
       </c>
-      <c r="AC12" s="1">
+      <c r="AC12">
         <v>15</v>
       </c>
-      <c r="AD12" s="4"/>
-      <c r="AE12" s="3" t="s">
+      <c r="AD12" s="2"/>
+      <c r="AE12" t="s">
         <v>52</v>
       </c>
-      <c r="AF12" s="3" t="s">
+      <c r="AF12" t="s">
         <v>53</v>
       </c>
-      <c r="AG12" s="3"/>
-      <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="3">
         <v>44362</v>
       </c>
-      <c r="C13" s="5">
+      <c r="C13" s="3">
         <v>44722</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13">
         <v>12</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13">
         <v>45</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13">
         <v>-97</v>
       </c>
-      <c r="G13" s="3">
-        <v>0</v>
-      </c>
-      <c r="H13" s="3">
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
         <v>-71</v>
       </c>
-      <c r="I13" s="3">
+      <c r="I13">
         <v>5</v>
       </c>
-      <c r="J13" s="3">
+      <c r="J13">
         <v>300</v>
       </c>
-      <c r="K13" s="3">
+      <c r="K13">
         <v>30</v>
       </c>
-      <c r="L13" s="3">
+      <c r="L13">
         <v>1</v>
       </c>
-      <c r="M13" s="3"/>
       <c r="N13">
         <v>0.9</v>
       </c>
@@ -2502,94 +2454,90 @@
       <c r="P13">
         <v>1.4</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13">
         <v>-82.304972000000006</v>
       </c>
-      <c r="R13" s="6">
+      <c r="R13">
         <v>37.286811999999998</v>
       </c>
-      <c r="S13" s="4">
+      <c r="S13" s="2">
         <v>44378</v>
       </c>
-      <c r="T13" s="4">
+      <c r="T13" s="2">
         <v>44454</v>
       </c>
-      <c r="U13" s="4">
+      <c r="U13" s="2">
         <v>44671</v>
       </c>
-      <c r="V13" s="4">
+      <c r="V13" s="2">
         <v>44722</v>
       </c>
-      <c r="W13" s="6">
+      <c r="W13">
         <v>-82.304972000000006</v>
       </c>
-      <c r="X13" s="6">
+      <c r="X13">
         <v>37.286811999999998</v>
       </c>
-      <c r="Y13" s="1">
+      <c r="Y13">
         <v>0.1</v>
       </c>
-      <c r="Z13" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA13" s="1">
+      <c r="Z13">
+        <v>0.9</v>
+      </c>
+      <c r="AA13">
         <v>120</v>
       </c>
-      <c r="AB13" s="1">
+      <c r="AB13">
         <v>100</v>
       </c>
-      <c r="AC13" s="1">
+      <c r="AC13">
         <v>15</v>
       </c>
-      <c r="AD13" s="4"/>
-      <c r="AE13" s="3" t="s">
+      <c r="AD13" s="2"/>
+      <c r="AE13" t="s">
         <v>52</v>
       </c>
-      <c r="AF13" s="3" t="s">
+      <c r="AF13" t="s">
         <v>53</v>
       </c>
-      <c r="AG13" s="3"/>
-      <c r="AH13" s="3"/>
-      <c r="AI13" s="3"/>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="3">
         <v>44362</v>
       </c>
-      <c r="C14" s="5">
+      <c r="C14" s="3">
         <v>44722</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14">
         <v>12</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14">
         <v>45</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14">
         <v>-97</v>
       </c>
-      <c r="G14" s="3">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
         <v>-71</v>
       </c>
-      <c r="I14" s="3">
+      <c r="I14">
         <v>5</v>
       </c>
-      <c r="J14" s="3">
+      <c r="J14">
         <v>300</v>
       </c>
-      <c r="K14" s="3">
+      <c r="K14">
         <v>30</v>
       </c>
-      <c r="L14" s="3">
+      <c r="L14">
         <v>1</v>
       </c>
-      <c r="M14" s="3"/>
       <c r="N14">
         <v>0.9</v>
       </c>
@@ -2599,94 +2547,90 @@
       <c r="P14">
         <v>1.4</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="Q14">
         <v>-82.305835000000002</v>
       </c>
-      <c r="R14" s="6">
+      <c r="R14">
         <v>37.293075999999999</v>
       </c>
-      <c r="S14" s="4">
+      <c r="S14" s="2">
         <v>44378</v>
       </c>
-      <c r="T14" s="4">
+      <c r="T14" s="2">
         <v>44454</v>
       </c>
-      <c r="U14" s="4">
+      <c r="U14" s="2">
         <v>44676</v>
       </c>
-      <c r="V14" s="4">
+      <c r="V14" s="2">
         <v>44722</v>
       </c>
-      <c r="W14" s="6">
+      <c r="W14">
         <v>-82.305835000000002</v>
       </c>
-      <c r="X14" s="6">
+      <c r="X14">
         <v>37.293075999999999</v>
       </c>
-      <c r="Y14" s="1">
+      <c r="Y14">
         <v>0.1</v>
       </c>
-      <c r="Z14" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA14" s="1">
+      <c r="Z14">
+        <v>0.9</v>
+      </c>
+      <c r="AA14">
         <v>120</v>
       </c>
-      <c r="AB14" s="1">
+      <c r="AB14">
         <v>100</v>
       </c>
-      <c r="AC14" s="1">
+      <c r="AC14">
         <v>15</v>
       </c>
-      <c r="AD14" s="4"/>
-      <c r="AE14" s="3" t="s">
+      <c r="AD14" s="2"/>
+      <c r="AE14" t="s">
         <v>52</v>
       </c>
-      <c r="AF14" s="3" t="s">
+      <c r="AF14" t="s">
         <v>53</v>
       </c>
-      <c r="AG14" s="3"/>
-      <c r="AH14" s="3"/>
-      <c r="AI14" s="3"/>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="3">
         <v>44362</v>
       </c>
-      <c r="C15" s="5">
+      <c r="C15" s="3">
         <v>44682</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15">
         <v>12</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15">
         <v>45</v>
       </c>
-      <c r="F15" s="3">
+      <c r="F15">
         <v>-97</v>
       </c>
-      <c r="G15" s="3">
-        <v>0</v>
-      </c>
-      <c r="H15" s="3">
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
         <v>-71</v>
       </c>
-      <c r="I15" s="3">
+      <c r="I15">
         <v>5</v>
       </c>
-      <c r="J15" s="3">
+      <c r="J15">
         <v>300</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K15">
         <v>30</v>
       </c>
-      <c r="L15" s="3">
+      <c r="L15">
         <v>1</v>
       </c>
-      <c r="M15" s="3"/>
       <c r="N15">
         <v>0.9</v>
       </c>
@@ -2696,94 +2640,90 @@
       <c r="P15">
         <v>1.4</v>
       </c>
-      <c r="Q15" s="6">
+      <c r="Q15">
         <v>-90.958820000000003</v>
       </c>
-      <c r="R15" s="6">
+      <c r="R15">
         <v>30.657959999999999</v>
       </c>
-      <c r="S15" s="4">
+      <c r="S15" s="2">
         <v>44363</v>
       </c>
-      <c r="T15" s="4">
+      <c r="T15" s="2">
         <v>44454</v>
       </c>
-      <c r="U15" s="4">
+      <c r="U15" s="2">
         <v>44662</v>
       </c>
-      <c r="V15" s="9">
+      <c r="V15" s="6">
         <v>44682</v>
       </c>
-      <c r="W15" s="6">
+      <c r="W15">
         <v>-90.958820000000003</v>
       </c>
-      <c r="X15" s="6">
+      <c r="X15">
         <v>30.657959999999999</v>
       </c>
-      <c r="Y15" s="1">
+      <c r="Y15">
         <v>0.1</v>
       </c>
-      <c r="Z15" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA15" s="1">
+      <c r="Z15">
+        <v>0.9</v>
+      </c>
+      <c r="AA15">
         <v>120</v>
       </c>
-      <c r="AB15" s="1">
+      <c r="AB15">
         <v>100</v>
       </c>
-      <c r="AC15" s="1">
+      <c r="AC15">
         <v>15</v>
       </c>
-      <c r="AD15" s="4"/>
-      <c r="AE15" s="3" t="s">
+      <c r="AD15" s="2"/>
+      <c r="AE15" t="s">
         <v>52</v>
       </c>
-      <c r="AF15" s="3" t="s">
+      <c r="AF15" t="s">
         <v>53</v>
       </c>
-      <c r="AG15" s="3"/>
-      <c r="AH15" s="3"/>
-      <c r="AI15" s="3"/>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="3">
         <v>44362</v>
       </c>
-      <c r="C16" s="5">
+      <c r="C16" s="3">
         <v>44666</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16">
         <v>12</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16">
         <v>45</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16">
         <v>-97</v>
       </c>
-      <c r="G16" s="3">
-        <v>0</v>
-      </c>
-      <c r="H16" s="3">
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
         <v>-71</v>
       </c>
-      <c r="I16" s="3">
+      <c r="I16">
         <v>5</v>
       </c>
-      <c r="J16" s="3">
+      <c r="J16">
         <v>300</v>
       </c>
-      <c r="K16" s="3">
+      <c r="K16">
         <v>30</v>
       </c>
-      <c r="L16" s="3">
+      <c r="L16">
         <v>1</v>
       </c>
-      <c r="M16" s="3"/>
       <c r="N16">
         <v>0.9</v>
       </c>
@@ -2793,94 +2733,90 @@
       <c r="P16">
         <v>1.4</v>
       </c>
-      <c r="Q16" s="6">
+      <c r="Q16">
         <v>30.473739999999999</v>
       </c>
-      <c r="R16" s="6">
+      <c r="R16">
         <v>-90.992949999999993</v>
       </c>
-      <c r="S16" s="4">
+      <c r="S16" s="2">
         <v>44363</v>
       </c>
-      <c r="T16" s="4">
+      <c r="T16" s="2">
         <v>44454</v>
       </c>
-      <c r="U16" s="4">
+      <c r="U16" s="2">
         <v>44652</v>
       </c>
-      <c r="V16" s="9">
+      <c r="V16" s="6">
         <v>44666</v>
       </c>
-      <c r="W16" s="6">
+      <c r="W16">
         <v>30.473739999999999</v>
       </c>
-      <c r="X16" s="6">
+      <c r="X16">
         <v>-90.992949999999993</v>
       </c>
-      <c r="Y16" s="1">
+      <c r="Y16">
         <v>0.1</v>
       </c>
-      <c r="Z16" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA16" s="1">
+      <c r="Z16">
+        <v>0.9</v>
+      </c>
+      <c r="AA16">
         <v>120</v>
       </c>
-      <c r="AB16" s="1">
+      <c r="AB16">
         <v>100</v>
       </c>
-      <c r="AC16" s="1">
+      <c r="AC16">
         <v>15</v>
       </c>
-      <c r="AD16" s="4"/>
-      <c r="AE16" s="3" t="s">
+      <c r="AD16" s="2"/>
+      <c r="AE16" t="s">
         <v>52</v>
       </c>
-      <c r="AF16" s="3" t="s">
+      <c r="AF16" t="s">
         <v>53</v>
       </c>
-      <c r="AG16" s="3"/>
-      <c r="AH16" s="3"/>
-      <c r="AI16" s="3"/>
     </row>
-    <row r="17" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A17" s="2" t="s">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B17" s="5">
+      <c r="B17" s="3">
         <v>44362</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="3">
         <v>44677</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17">
         <v>12</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17">
         <v>45</v>
       </c>
-      <c r="F17" s="3">
+      <c r="F17">
         <v>-97</v>
       </c>
-      <c r="G17" s="3">
-        <v>0</v>
-      </c>
-      <c r="H17" s="3">
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
         <v>-71</v>
       </c>
-      <c r="I17" s="3">
+      <c r="I17">
         <v>5</v>
       </c>
-      <c r="J17" s="3">
+      <c r="J17">
         <v>300</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K17">
         <v>30</v>
       </c>
-      <c r="L17" s="3">
+      <c r="L17">
         <v>1</v>
       </c>
-      <c r="M17" s="3"/>
       <c r="N17">
         <v>0.9</v>
       </c>
@@ -2890,94 +2826,90 @@
       <c r="P17">
         <v>1.4</v>
       </c>
-      <c r="Q17" s="6">
+      <c r="Q17">
         <v>-91.364180000000005</v>
       </c>
-      <c r="R17" s="6">
+      <c r="R17">
         <v>30.418990000000001</v>
       </c>
-      <c r="S17" s="4">
+      <c r="S17" s="2">
         <v>44349</v>
       </c>
-      <c r="T17" s="4">
+      <c r="T17" s="2">
         <v>44454</v>
       </c>
-      <c r="U17" s="4">
+      <c r="U17" s="2">
         <v>44655</v>
       </c>
-      <c r="V17" s="9">
+      <c r="V17" s="6">
         <v>44677</v>
       </c>
-      <c r="W17" s="6">
+      <c r="W17">
         <v>-91.364180000000005</v>
       </c>
-      <c r="X17" s="6">
+      <c r="X17">
         <v>30.418990000000001</v>
       </c>
-      <c r="Y17" s="1">
+      <c r="Y17">
         <v>0.1</v>
       </c>
-      <c r="Z17" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA17" s="1">
+      <c r="Z17">
+        <v>0.9</v>
+      </c>
+      <c r="AA17">
         <v>120</v>
       </c>
-      <c r="AB17" s="1">
+      <c r="AB17">
         <v>100</v>
       </c>
-      <c r="AC17" s="1">
+      <c r="AC17">
         <v>15</v>
       </c>
-      <c r="AD17" s="4"/>
-      <c r="AE17" s="3" t="s">
+      <c r="AD17" s="2"/>
+      <c r="AE17" t="s">
         <v>52</v>
       </c>
-      <c r="AF17" s="3" t="s">
+      <c r="AF17" t="s">
         <v>53</v>
       </c>
-      <c r="AG17" s="3"/>
-      <c r="AH17" s="3"/>
-      <c r="AI17" s="3"/>
     </row>
-    <row r="18" spans="1:35" x14ac:dyDescent="0.35">
-      <c r="A18" s="2" t="s">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="B18" s="5">
+      <c r="B18" s="3">
         <v>44362</v>
       </c>
-      <c r="C18" s="5">
+      <c r="C18" s="3">
         <v>44684</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18">
         <v>12</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18">
         <v>45</v>
       </c>
-      <c r="F18" s="3">
+      <c r="F18">
         <v>-97</v>
       </c>
-      <c r="G18" s="3">
-        <v>0</v>
-      </c>
-      <c r="H18" s="3">
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
         <v>-71</v>
       </c>
-      <c r="I18" s="3">
+      <c r="I18">
         <v>5</v>
       </c>
-      <c r="J18" s="3">
+      <c r="J18">
         <v>300</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K18">
         <v>30</v>
       </c>
-      <c r="L18" s="3">
+      <c r="L18">
         <v>1</v>
       </c>
-      <c r="M18" s="3"/>
       <c r="N18">
         <v>0.9</v>
       </c>
@@ -2987,55 +2919,52 @@
       <c r="P18">
         <v>1.4</v>
       </c>
-      <c r="Q18" s="6">
+      <c r="Q18">
         <v>-91.371089999999995</v>
       </c>
-      <c r="R18" s="6">
+      <c r="R18">
         <v>30.415649999999999</v>
       </c>
-      <c r="S18" s="4">
+      <c r="S18" s="2">
         <v>44343</v>
       </c>
-      <c r="T18" s="4">
+      <c r="T18" s="2">
         <v>44454</v>
       </c>
-      <c r="U18" s="4">
+      <c r="U18" s="2">
         <v>44659</v>
       </c>
-      <c r="V18" s="9">
+      <c r="V18" s="6">
         <v>44684</v>
       </c>
-      <c r="W18" s="6">
+      <c r="W18">
         <v>-91.371089999999995</v>
       </c>
-      <c r="X18" s="6">
+      <c r="X18">
         <v>30.415649999999999</v>
       </c>
-      <c r="Y18" s="1">
+      <c r="Y18">
         <v>0.1</v>
       </c>
-      <c r="Z18" s="1">
-        <v>0.9</v>
-      </c>
-      <c r="AA18" s="1">
+      <c r="Z18">
+        <v>0.9</v>
+      </c>
+      <c r="AA18">
         <v>120</v>
       </c>
-      <c r="AB18" s="1">
+      <c r="AB18">
         <v>100</v>
       </c>
-      <c r="AC18" s="1">
+      <c r="AC18">
         <v>15</v>
       </c>
-      <c r="AD18" s="4"/>
-      <c r="AE18" s="3" t="s">
+      <c r="AD18" s="2"/>
+      <c r="AE18" t="s">
         <v>52</v>
       </c>
-      <c r="AF18" s="3" t="s">
+      <c r="AF18" t="s">
         <v>53</v>
       </c>
-      <c r="AG18" s="3"/>
-      <c r="AH18" s="3"/>
-      <c r="AI18" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>

<commit_message>
More tag commits (Sept 7)
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett Rhyne\Documents\SWWA_Connectivity\Analysis\SWWA_Pressure\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599D2EAB-7BDA-4512-84AE-9E355182E837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19CAFF5-54CF-40AA-93B4-03AC1ADF2542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30330" yWindow="3810" windowWidth="22440" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="9260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tracks" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
   <si>
     <t>mass</t>
   </si>
@@ -163,9 +163,6 @@
   </si>
   <si>
     <t>CB611</t>
-  </si>
-  <si>
-    <t>CB613</t>
   </si>
   <si>
     <t>CB616</t>
@@ -898,8 +895,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AI18" totalsRowShown="0">
-  <autoFilter ref="A1:AI18" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}" name="Table1" displayName="Table1" ref="A1:AI17" totalsRowShown="0">
+  <autoFilter ref="A1:AI17" xr:uid="{3E83695E-4F69-0542-A434-9A92AEDC21B8}"/>
   <tableColumns count="35">
     <tableColumn id="3" xr3:uid="{0E08F938-60A9-C640-A060-C64653A1D0F0}" name="gdl_id" dataDxfId="16" dataCellStyle="Normal_Feuil1"/>
     <tableColumn id="38" xr3:uid="{5F80A124-B607-6D47-A8B2-B6EBC16D0EC2}" name="crop_start"/>
@@ -1238,10 +1235,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI18"/>
+  <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15:X15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1472,10 +1469,10 @@
       </c>
       <c r="AD2" s="2"/>
       <c r="AE2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF2" t="s">
         <v>52</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.35">
@@ -1565,10 +1562,10 @@
       </c>
       <c r="AD3" s="2"/>
       <c r="AE3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF3" t="s">
         <v>52</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.35">
@@ -1658,10 +1655,10 @@
       </c>
       <c r="AD4" s="2"/>
       <c r="AE4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF4" t="s">
         <v>52</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.35">
@@ -1751,10 +1748,10 @@
       </c>
       <c r="AD5" s="2"/>
       <c r="AE5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF5" t="s">
         <v>52</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.35">
@@ -1844,10 +1841,10 @@
       </c>
       <c r="AD6" s="2"/>
       <c r="AE6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF6" t="s">
         <v>52</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.35">
@@ -1937,10 +1934,10 @@
       </c>
       <c r="AD7" s="2"/>
       <c r="AE7" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF7" t="s">
         <v>52</v>
-      </c>
-      <c r="AF7" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.35">
@@ -2030,10 +2027,10 @@
       </c>
       <c r="AD8" s="2"/>
       <c r="AE8" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF8" t="s">
         <v>52</v>
-      </c>
-      <c r="AF8" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:35" x14ac:dyDescent="0.35">
@@ -2123,10 +2120,10 @@
       </c>
       <c r="AD9" s="2"/>
       <c r="AE9" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF9" t="s">
         <v>52</v>
-      </c>
-      <c r="AF9" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.35">
@@ -2216,10 +2213,10 @@
       </c>
       <c r="AD10" s="2"/>
       <c r="AE10" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF10" t="s">
         <v>52</v>
-      </c>
-      <c r="AF10" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:35" x14ac:dyDescent="0.35">
@@ -2230,7 +2227,7 @@
         <v>44362</v>
       </c>
       <c r="C11" s="3">
-        <v>44685</v>
+        <v>44726</v>
       </c>
       <c r="D11">
         <v>12</v>
@@ -2269,28 +2266,28 @@
         <v>1.4</v>
       </c>
       <c r="Q11">
-        <v>-91.214569999999995</v>
+        <v>-82.301767999999996</v>
       </c>
       <c r="R11">
-        <v>36.732098999999998</v>
+        <v>37.294294999999998</v>
       </c>
       <c r="S11" s="2">
-        <v>44363</v>
+        <v>44378</v>
       </c>
       <c r="T11" s="2">
         <v>44454</v>
       </c>
       <c r="U11" s="2">
-        <v>44666</v>
+        <v>44671</v>
       </c>
       <c r="V11" s="2">
-        <v>44685</v>
+        <v>44726</v>
       </c>
       <c r="W11">
-        <v>-91.214569999999995</v>
+        <v>-82.301767999999996</v>
       </c>
       <c r="X11">
-        <v>36.732098999999998</v>
+        <v>37.294294999999998</v>
       </c>
       <c r="Y11">
         <v>0.1</v>
@@ -2309,10 +2306,10 @@
       </c>
       <c r="AD11" s="2"/>
       <c r="AE11" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF11" t="s">
         <v>52</v>
-      </c>
-      <c r="AF11" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:35" x14ac:dyDescent="0.35">
@@ -2323,7 +2320,7 @@
         <v>44362</v>
       </c>
       <c r="C12" s="3">
-        <v>44726</v>
+        <v>44722</v>
       </c>
       <c r="D12">
         <v>12</v>
@@ -2362,10 +2359,10 @@
         <v>1.4</v>
       </c>
       <c r="Q12">
-        <v>-82.301767999999996</v>
+        <v>-82.304972000000006</v>
       </c>
       <c r="R12">
-        <v>37.294294999999998</v>
+        <v>37.286811999999998</v>
       </c>
       <c r="S12" s="2">
         <v>44378</v>
@@ -2377,13 +2374,13 @@
         <v>44671</v>
       </c>
       <c r="V12" s="2">
-        <v>44726</v>
+        <v>44722</v>
       </c>
       <c r="W12">
-        <v>-82.301767999999996</v>
+        <v>-82.304972000000006</v>
       </c>
       <c r="X12">
-        <v>37.294294999999998</v>
+        <v>37.286811999999998</v>
       </c>
       <c r="Y12">
         <v>0.1</v>
@@ -2402,10 +2399,10 @@
       </c>
       <c r="AD12" s="2"/>
       <c r="AE12" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF12" t="s">
         <v>52</v>
-      </c>
-      <c r="AF12" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="13" spans="1:35" x14ac:dyDescent="0.35">
@@ -2455,10 +2452,10 @@
         <v>1.4</v>
       </c>
       <c r="Q13">
-        <v>-82.304972000000006</v>
+        <v>-82.305835000000002</v>
       </c>
       <c r="R13">
-        <v>37.286811999999998</v>
+        <v>37.293075999999999</v>
       </c>
       <c r="S13" s="2">
         <v>44378</v>
@@ -2467,16 +2464,16 @@
         <v>44454</v>
       </c>
       <c r="U13" s="2">
-        <v>44671</v>
+        <v>44676</v>
       </c>
       <c r="V13" s="2">
         <v>44722</v>
       </c>
       <c r="W13">
-        <v>-82.304972000000006</v>
+        <v>-82.305835000000002</v>
       </c>
       <c r="X13">
-        <v>37.286811999999998</v>
+        <v>37.293075999999999</v>
       </c>
       <c r="Y13">
         <v>0.1</v>
@@ -2495,10 +2492,10 @@
       </c>
       <c r="AD13" s="2"/>
       <c r="AE13" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF13" t="s">
         <v>52</v>
-      </c>
-      <c r="AF13" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.35">
@@ -2509,7 +2506,7 @@
         <v>44362</v>
       </c>
       <c r="C14" s="3">
-        <v>44722</v>
+        <v>44682</v>
       </c>
       <c r="D14">
         <v>12</v>
@@ -2548,28 +2545,28 @@
         <v>1.4</v>
       </c>
       <c r="Q14">
-        <v>-82.305835000000002</v>
+        <v>-90.958820000000003</v>
       </c>
       <c r="R14">
-        <v>37.293075999999999</v>
+        <v>30.657959999999999</v>
       </c>
       <c r="S14" s="2">
-        <v>44378</v>
+        <v>44363</v>
       </c>
       <c r="T14" s="2">
         <v>44454</v>
       </c>
       <c r="U14" s="2">
-        <v>44676</v>
-      </c>
-      <c r="V14" s="2">
-        <v>44722</v>
+        <v>44662</v>
+      </c>
+      <c r="V14" s="6">
+        <v>44682</v>
       </c>
       <c r="W14">
-        <v>-82.305835000000002</v>
+        <v>-90.958820000000003</v>
       </c>
       <c r="X14">
-        <v>37.293075999999999</v>
+        <v>30.657959999999999</v>
       </c>
       <c r="Y14">
         <v>0.1</v>
@@ -2588,10 +2585,10 @@
       </c>
       <c r="AD14" s="2"/>
       <c r="AE14" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF14" t="s">
         <v>52</v>
-      </c>
-      <c r="AF14" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:35" x14ac:dyDescent="0.35">
@@ -2602,7 +2599,7 @@
         <v>44362</v>
       </c>
       <c r="C15" s="3">
-        <v>44682</v>
+        <v>44666</v>
       </c>
       <c r="D15">
         <v>12</v>
@@ -2641,10 +2638,10 @@
         <v>1.4</v>
       </c>
       <c r="Q15">
-        <v>-90.958820000000003</v>
+        <v>-90.992949999999993</v>
       </c>
       <c r="R15">
-        <v>30.657959999999999</v>
+        <v>30.473739999999999</v>
       </c>
       <c r="S15" s="2">
         <v>44363</v>
@@ -2653,16 +2650,16 @@
         <v>44454</v>
       </c>
       <c r="U15" s="2">
-        <v>44662</v>
+        <v>44652</v>
       </c>
       <c r="V15" s="6">
-        <v>44682</v>
+        <v>44666</v>
       </c>
       <c r="W15">
-        <v>-90.958820000000003</v>
+        <v>-90.992949999999993</v>
       </c>
       <c r="X15">
-        <v>30.657959999999999</v>
+        <v>30.473739999999999</v>
       </c>
       <c r="Y15">
         <v>0.1</v>
@@ -2671,7 +2668,7 @@
         <v>0.9</v>
       </c>
       <c r="AA15">
-        <v>120</v>
+        <v>200</v>
       </c>
       <c r="AB15">
         <v>100</v>
@@ -2681,10 +2678,10 @@
       </c>
       <c r="AD15" s="2"/>
       <c r="AE15" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF15" t="s">
         <v>52</v>
-      </c>
-      <c r="AF15" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:35" x14ac:dyDescent="0.35">
@@ -2695,7 +2692,7 @@
         <v>44362</v>
       </c>
       <c r="C16" s="3">
-        <v>44666</v>
+        <v>44677</v>
       </c>
       <c r="D16">
         <v>12</v>
@@ -2734,28 +2731,28 @@
         <v>1.4</v>
       </c>
       <c r="Q16">
-        <v>30.473739999999999</v>
+        <v>-91.364180000000005</v>
       </c>
       <c r="R16">
-        <v>-90.992949999999993</v>
+        <v>30.418990000000001</v>
       </c>
       <c r="S16" s="2">
-        <v>44363</v>
+        <v>44349</v>
       </c>
       <c r="T16" s="2">
         <v>44454</v>
       </c>
       <c r="U16" s="2">
-        <v>44652</v>
+        <v>44655</v>
       </c>
       <c r="V16" s="6">
-        <v>44666</v>
+        <v>44677</v>
       </c>
       <c r="W16">
-        <v>30.473739999999999</v>
+        <v>-91.364180000000005</v>
       </c>
       <c r="X16">
-        <v>-90.992949999999993</v>
+        <v>30.418990000000001</v>
       </c>
       <c r="Y16">
         <v>0.1</v>
@@ -2774,10 +2771,10 @@
       </c>
       <c r="AD16" s="2"/>
       <c r="AE16" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF16" t="s">
         <v>52</v>
-      </c>
-      <c r="AF16" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="17" spans="1:32" x14ac:dyDescent="0.35">
@@ -2788,7 +2785,7 @@
         <v>44362</v>
       </c>
       <c r="C17" s="3">
-        <v>44677</v>
+        <v>44684</v>
       </c>
       <c r="D17">
         <v>12</v>
@@ -2827,28 +2824,28 @@
         <v>1.4</v>
       </c>
       <c r="Q17">
-        <v>-91.364180000000005</v>
+        <v>-91.371089999999995</v>
       </c>
       <c r="R17">
-        <v>30.418990000000001</v>
+        <v>30.415649999999999</v>
       </c>
       <c r="S17" s="2">
-        <v>44349</v>
+        <v>44343</v>
       </c>
       <c r="T17" s="2">
         <v>44454</v>
       </c>
       <c r="U17" s="2">
-        <v>44655</v>
+        <v>44659</v>
       </c>
       <c r="V17" s="6">
-        <v>44677</v>
+        <v>44684</v>
       </c>
       <c r="W17">
-        <v>-91.364180000000005</v>
+        <v>-91.371089999999995</v>
       </c>
       <c r="X17">
-        <v>30.418990000000001</v>
+        <v>30.415649999999999</v>
       </c>
       <c r="Y17">
         <v>0.1</v>
@@ -2867,103 +2864,10 @@
       </c>
       <c r="AD17" s="2"/>
       <c r="AE17" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF17" t="s">
         <v>52</v>
-      </c>
-      <c r="AF17" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.35">
-      <c r="A18" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="B18" s="3">
-        <v>44362</v>
-      </c>
-      <c r="C18" s="3">
-        <v>44684</v>
-      </c>
-      <c r="D18">
-        <v>12</v>
-      </c>
-      <c r="E18">
-        <v>45</v>
-      </c>
-      <c r="F18">
-        <v>-97</v>
-      </c>
-      <c r="G18">
-        <v>0</v>
-      </c>
-      <c r="H18">
-        <v>-71</v>
-      </c>
-      <c r="I18">
-        <v>5</v>
-      </c>
-      <c r="J18">
-        <v>300</v>
-      </c>
-      <c r="K18">
-        <v>30</v>
-      </c>
-      <c r="L18">
-        <v>1</v>
-      </c>
-      <c r="N18">
-        <v>0.9</v>
-      </c>
-      <c r="O18">
-        <v>0</v>
-      </c>
-      <c r="P18">
-        <v>1.4</v>
-      </c>
-      <c r="Q18">
-        <v>-91.371089999999995</v>
-      </c>
-      <c r="R18">
-        <v>30.415649999999999</v>
-      </c>
-      <c r="S18" s="2">
-        <v>44343</v>
-      </c>
-      <c r="T18" s="2">
-        <v>44454</v>
-      </c>
-      <c r="U18" s="2">
-        <v>44659</v>
-      </c>
-      <c r="V18" s="6">
-        <v>44684</v>
-      </c>
-      <c r="W18">
-        <v>-91.371089999999995</v>
-      </c>
-      <c r="X18">
-        <v>30.415649999999999</v>
-      </c>
-      <c r="Y18">
-        <v>0.1</v>
-      </c>
-      <c r="Z18">
-        <v>0.9</v>
-      </c>
-      <c r="AA18">
-        <v>120</v>
-      </c>
-      <c r="AB18">
-        <v>100</v>
-      </c>
-      <c r="AC18">
-        <v>15</v>
-      </c>
-      <c r="AD18" s="2"/>
-      <c r="AE18" t="s">
-        <v>52</v>
-      </c>
-      <c r="AF18" t="s">
-        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update gpr dur_thr for 2 tags
</commit_message>
<xml_diff>
--- a/data/gpr_settings.xlsx
+++ b/data/gpr_settings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Garrett Rhyne\Documents\SWWA_Connectivity\Analysis\SWWA_Pressure\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19CAFF5-54CF-40AA-93B4-03AC1ADF2542}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B4C29B5-7CDD-49F0-9AF5-226863EEABBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="760" windowWidth="14400" windowHeight="9260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1237,8 +1237,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15:X15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1579,7 +1579,7 @@
         <v>44721</v>
       </c>
       <c r="D4">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="E4">
         <v>45</v>
@@ -2230,7 +2230,7 @@
         <v>44726</v>
       </c>
       <c r="D11">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="E11">
         <v>45</v>

</xml_diff>